<commit_message>
initailize the BRD structure
</commit_message>
<xml_diff>
--- a/01_doc/proj_plan/餐厅订餐系统_项目计划.xlsx
+++ b/01_doc/proj_plan/餐厅订餐系统_项目计划.xlsx
@@ -1244,8 +1244,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1390,12 +1388,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1405,15 +1397,23 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2315,7 +2315,7 @@
       <c r="A2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="40">
+      <c r="B2" s="38">
         <v>41962</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2332,7 +2332,7 @@
       <c r="A3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="38">
         <v>41963</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2349,7 +2349,7 @@
       <c r="A4" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="38">
         <v>41963</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -2459,7 +2459,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="33" t="s">
         <v>114</v>
       </c>
       <c r="B12" t="s">
@@ -2473,7 +2473,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="33" t="s">
         <v>115</v>
       </c>
       <c r="B13" t="s">
@@ -2487,7 +2487,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="33" t="s">
         <v>116</v>
       </c>
       <c r="B14" t="s">
@@ -2608,8 +2608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:M27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2620,700 +2620,700 @@
   <sheetData>
     <row r="1" spans="2:13" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="53"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="51"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="56"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="54"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="56"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="54"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="56"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="54"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="53"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="51"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="56"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="54"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="56"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="54"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="56"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="54"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="57"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="59"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="57"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="61"/>
-      <c r="M14" s="62"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="60"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="65"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="63"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="63"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="65"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="63"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="65"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="63"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="65"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="63"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="63"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="64"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="64"/>
-      <c r="M19" s="65"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="63"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="63"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="65"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="63"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="63"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="65"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="63"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="63"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="65"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="63"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="63"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="64"/>
-      <c r="M23" s="65"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="63"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="63"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="65"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="63"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="63"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="65"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="63"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="63"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="65"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="63"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="66"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="67"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="68"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="66"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="51" t="s">
+      <c r="B28" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="44"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="42"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="47"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="45"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="45"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="47"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="45"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="45"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="47"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="44"/>
+      <c r="M32" s="45"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="45"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="47"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="45"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="45"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="46"/>
-      <c r="M34" s="47"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="44"/>
+      <c r="M34" s="45"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="48"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="50"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="48"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="51"/>
-      <c r="M36" s="51"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="69"/>
-      <c r="L37" s="69"/>
-      <c r="M37" s="70"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="67"/>
+      <c r="M37" s="68"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="71"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="72"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="73"/>
+      <c r="B38" s="69"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="70"/>
+      <c r="J38" s="70"/>
+      <c r="K38" s="70"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="71"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="71"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="72"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="72"/>
-      <c r="M39" s="73"/>
+      <c r="B39" s="69"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
+      <c r="K39" s="70"/>
+      <c r="L39" s="70"/>
+      <c r="M39" s="71"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="71"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
-      <c r="F40" s="72"/>
-      <c r="G40" s="72"/>
-      <c r="H40" s="72"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="72"/>
-      <c r="K40" s="72"/>
-      <c r="L40" s="72"/>
-      <c r="M40" s="73"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="70"/>
+      <c r="J40" s="70"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="70"/>
+      <c r="M40" s="71"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="74"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
-      <c r="M41" s="76"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="73"/>
+      <c r="I41" s="73"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="73"/>
+      <c r="M41" s="74"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
-      <c r="M43" s="44"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="41"/>
+      <c r="L43" s="41"/>
+      <c r="M43" s="42"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="45"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
-      <c r="K44" s="46"/>
-      <c r="L44" s="46"/>
-      <c r="M44" s="47"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+      <c r="M44" s="45"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="45"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="47"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
+      <c r="M45" s="45"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="47"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="44"/>
+      <c r="M46" s="45"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="45"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="46"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="46"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="46"/>
-      <c r="M47" s="47"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="44"/>
+      <c r="M47" s="45"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="45"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="46"/>
-      <c r="H48" s="46"/>
-      <c r="I48" s="46"/>
-      <c r="J48" s="46"/>
-      <c r="K48" s="46"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="47"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="44"/>
+      <c r="M48" s="45"/>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="48"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="49"/>
-      <c r="I49" s="49"/>
-      <c r="J49" s="49"/>
-      <c r="K49" s="49"/>
-      <c r="L49" s="49"/>
-      <c r="M49" s="50"/>
+      <c r="B49" s="46"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="47"/>
+      <c r="J49" s="47"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="47"/>
+      <c r="M49" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3362,10 +3362,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
       <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
@@ -3380,10 +3380,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="77">
+      <c r="A3" s="75">
         <v>1</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="75" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="7">
@@ -3406,8 +3406,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="77"/>
-      <c r="B4" s="77"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="7">
         <v>1.2</v>
       </c>
@@ -3428,8 +3428,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="7">
         <v>1.3</v>
       </c>
@@ -3450,8 +3450,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="7">
         <v>1.4</v>
       </c>
@@ -3472,10 +3472,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="79">
+      <c r="A7" s="77">
         <v>2</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="75" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="7">
@@ -3498,8 +3498,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="80"/>
-      <c r="B8" s="77"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="7">
         <v>2.2000000000000002</v>
       </c>
@@ -3520,8 +3520,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="81"/>
-      <c r="B9" s="77"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="75"/>
       <c r="C9" s="7">
         <v>2.2999999999999998</v>
       </c>
@@ -3542,10 +3542,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="77">
+      <c r="A10" s="75">
         <v>3</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="75" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="9">
@@ -3568,8 +3568,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="77"/>
-      <c r="B11" s="77"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="9">
         <v>3.2</v>
       </c>
@@ -3590,8 +3590,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="77"/>
-      <c r="B12" s="77"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="9">
         <v>3.3</v>
       </c>
@@ -3612,8 +3612,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="77"/>
-      <c r="B13" s="77"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="9">
         <v>3.4</v>
       </c>
@@ -3634,8 +3634,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="77"/>
-      <c r="B14" s="77"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="9">
         <v>3.5</v>
       </c>
@@ -3656,8 +3656,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="77"/>
-      <c r="B15" s="77"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="9">
         <v>3.6</v>
       </c>
@@ -3678,8 +3678,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="77"/>
-      <c r="B16" s="77"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="9">
         <v>3.7</v>
       </c>
@@ -3700,8 +3700,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="77"/>
-      <c r="B17" s="77"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="9">
         <v>3.8</v>
       </c>
@@ -3722,8 +3722,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="77"/>
-      <c r="B18" s="77"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="9">
         <v>3.9</v>
       </c>
@@ -3744,8 +3744,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="9" t="s">
         <v>51</v>
       </c>
@@ -3766,8 +3766,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="9">
         <v>3.11</v>
       </c>
@@ -3788,8 +3788,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="9">
         <v>3.12</v>
       </c>
@@ -3810,10 +3810,10 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="77">
+      <c r="A22" s="75">
         <v>4</v>
       </c>
-      <c r="B22" s="79" t="s">
+      <c r="B22" s="77" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="7">
@@ -3836,8 +3836,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23" s="77"/>
-      <c r="B23" s="80"/>
+      <c r="A23" s="75"/>
+      <c r="B23" s="78"/>
       <c r="C23" s="7">
         <v>4.2</v>
       </c>
@@ -3858,8 +3858,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="77"/>
-      <c r="B24" s="80"/>
+      <c r="A24" s="75"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="7">
         <v>4.3</v>
       </c>
@@ -3880,8 +3880,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="77"/>
-      <c r="B25" s="80"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="78"/>
       <c r="C25" s="7">
         <v>4.4000000000000004</v>
       </c>
@@ -3902,8 +3902,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="77"/>
-      <c r="B26" s="80"/>
+      <c r="A26" s="75"/>
+      <c r="B26" s="78"/>
       <c r="C26" s="7">
         <v>4.5</v>
       </c>
@@ -3924,8 +3924,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A27" s="77"/>
-      <c r="B27" s="80"/>
+      <c r="A27" s="75"/>
+      <c r="B27" s="78"/>
       <c r="C27" s="7">
         <v>4.5999999999999996</v>
       </c>
@@ -3946,8 +3946,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="77"/>
-      <c r="B28" s="80"/>
+      <c r="A28" s="75"/>
+      <c r="B28" s="78"/>
       <c r="C28" s="7">
         <v>4.7</v>
       </c>
@@ -3968,8 +3968,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="77"/>
-      <c r="B29" s="80"/>
+      <c r="A29" s="75"/>
+      <c r="B29" s="78"/>
       <c r="C29" s="7">
         <v>4.8</v>
       </c>
@@ -3990,10 +3990,10 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="77">
+      <c r="A30" s="75">
         <v>5</v>
       </c>
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="75" t="s">
         <v>63</v>
       </c>
       <c r="C30" s="7">
@@ -4016,8 +4016,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A31" s="77"/>
-      <c r="B31" s="77"/>
+      <c r="A31" s="75"/>
+      <c r="B31" s="75"/>
       <c r="C31" s="7">
         <v>5.2</v>
       </c>
@@ -4038,8 +4038,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="77"/>
-      <c r="B32" s="77"/>
+      <c r="A32" s="75"/>
+      <c r="B32" s="75"/>
       <c r="C32" s="7">
         <v>5.3</v>
       </c>
@@ -4060,8 +4060,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A33" s="77"/>
-      <c r="B33" s="77"/>
+      <c r="A33" s="75"/>
+      <c r="B33" s="75"/>
       <c r="C33" s="7">
         <v>5.4</v>
       </c>
@@ -4082,8 +4082,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="77"/>
-      <c r="B34" s="77"/>
+      <c r="A34" s="75"/>
+      <c r="B34" s="75"/>
       <c r="C34" s="7">
         <v>5.5</v>
       </c>
@@ -4104,8 +4104,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A35" s="77"/>
-      <c r="B35" s="77"/>
+      <c r="A35" s="75"/>
+      <c r="B35" s="75"/>
       <c r="C35" s="7">
         <v>5.6</v>
       </c>
@@ -4126,8 +4126,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A36" s="77"/>
-      <c r="B36" s="77"/>
+      <c r="A36" s="75"/>
+      <c r="B36" s="75"/>
       <c r="C36" s="7">
         <v>5.7</v>
       </c>
@@ -4148,10 +4148,10 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A37" s="77">
+      <c r="A37" s="75">
         <v>6</v>
       </c>
-      <c r="B37" s="77" t="s">
+      <c r="B37" s="75" t="s">
         <v>72</v>
       </c>
       <c r="C37" s="7">
@@ -4174,8 +4174,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A38" s="77"/>
-      <c r="B38" s="77"/>
+      <c r="A38" s="75"/>
+      <c r="B38" s="75"/>
       <c r="C38" s="7">
         <v>6.2</v>
       </c>
@@ -4196,8 +4196,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39" s="77"/>
-      <c r="B39" s="77"/>
+      <c r="A39" s="75"/>
+      <c r="B39" s="75"/>
       <c r="C39" s="7">
         <v>6.3</v>
       </c>
@@ -4218,8 +4218,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="77"/>
-      <c r="B40" s="77"/>
+      <c r="A40" s="75"/>
+      <c r="B40" s="75"/>
       <c r="C40" s="7">
         <v>6.4</v>
       </c>
@@ -4240,8 +4240,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
+      <c r="A41" s="75"/>
+      <c r="B41" s="75"/>
       <c r="C41" s="7">
         <v>6.5</v>
       </c>
@@ -4262,8 +4262,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A42" s="77"/>
-      <c r="B42" s="77"/>
+      <c r="A42" s="75"/>
+      <c r="B42" s="75"/>
       <c r="C42" s="7">
         <v>6.6</v>
       </c>
@@ -4602,7 +4602,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4614,60 +4614,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="88"/>
-      <c r="B1" s="88"/>
-      <c r="C1" s="87" t="s">
+      <c r="A1" s="83"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="84" t="s">
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="85"/>
-      <c r="Z1" s="85"/>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="85"/>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="85"/>
-      <c r="AF1" s="85"/>
-      <c r="AG1" s="85"/>
-      <c r="AH1" s="85"/>
-      <c r="AI1" s="85"/>
-      <c r="AJ1" s="85"/>
-      <c r="AK1" s="85"/>
-      <c r="AL1" s="85"/>
-      <c r="AM1" s="85"/>
-      <c r="AN1" s="85"/>
-      <c r="AO1" s="85"/>
-      <c r="AP1" s="85"/>
-      <c r="AQ1" s="85"/>
-      <c r="AR1" s="85"/>
-      <c r="AS1" s="85"/>
-      <c r="AT1" s="86"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81"/>
+      <c r="X1" s="81"/>
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
+      <c r="AE1" s="81"/>
+      <c r="AF1" s="81"/>
+      <c r="AG1" s="81"/>
+      <c r="AH1" s="81"/>
+      <c r="AI1" s="81"/>
+      <c r="AJ1" s="81"/>
+      <c r="AK1" s="81"/>
+      <c r="AL1" s="81"/>
+      <c r="AM1" s="81"/>
+      <c r="AN1" s="81"/>
+      <c r="AO1" s="81"/>
+      <c r="AP1" s="81"/>
+      <c r="AQ1" s="81"/>
+      <c r="AR1" s="81"/>
+      <c r="AS1" s="81"/>
+      <c r="AT1" s="82"/>
     </row>
     <row r="2" spans="1:60" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
       <c r="C2" s="16">
         <v>18</v>
       </c>
@@ -4820,9 +4820,9 @@
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -4864,7 +4864,7 @@
       <c r="AR3" s="19"/>
       <c r="AS3" s="19"/>
       <c r="AT3" s="19"/>
-      <c r="BG3" s="36"/>
+      <c r="BG3" s="34"/>
       <c r="BH3" s="4" t="s">
         <v>130</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="20"/>
-      <c r="D4" s="25"/>
+      <c r="D4" s="88"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
@@ -4920,7 +4920,7 @@
       <c r="AR4" s="19"/>
       <c r="AS4" s="19"/>
       <c r="AT4" s="19"/>
-      <c r="BG4" s="37"/>
+      <c r="BG4" s="35"/>
       <c r="BH4" s="4" t="s">
         <v>131</v>
       </c>
@@ -4932,7 +4932,7 @@
       <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="21"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
@@ -4976,7 +4976,7 @@
       <c r="AR5" s="19"/>
       <c r="AS5" s="19"/>
       <c r="AT5" s="19"/>
-      <c r="BG5" s="38"/>
+      <c r="BG5" s="36"/>
       <c r="BH5" s="4" t="s">
         <v>132</v>
       </c>
@@ -4989,8 +4989,8 @@
         <v>25</v>
       </c>
       <c r="C6" s="20"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="89"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
@@ -5032,21 +5032,21 @@
       <c r="AR6" s="19"/>
       <c r="AS6" s="19"/>
       <c r="AT6" s="19"/>
-      <c r="BG6" s="39"/>
+      <c r="BG6" s="37"/>
       <c r="BH6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:60" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="27" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
-      <c r="F7" s="30"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -5193,10 +5193,10 @@
       <c r="AT9" s="19"/>
     </row>
     <row r="10" spans="1:60" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="27" t="s">
         <v>85</v>
       </c>
       <c r="C10" s="20"/>
@@ -5204,7 +5204,7 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="I10" s="30"/>
+      <c r="I10" s="28"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
@@ -5512,8 +5512,8 @@
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
@@ -5575,7 +5575,7 @@
       <c r="M17" s="19"/>
       <c r="N17" s="19"/>
       <c r="O17" s="19"/>
-      <c r="Q17" s="30"/>
+      <c r="Q17" s="28"/>
       <c r="R17" s="19"/>
       <c r="S17" s="19"/>
       <c r="T17" s="19"/>
@@ -5763,10 +5763,10 @@
       <c r="AT20" s="19"/>
     </row>
     <row r="21" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="33">
+      <c r="A21" s="31">
         <v>3.9</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="30" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="20"/>
@@ -5815,10 +5815,10 @@
       <c r="AT21" s="19"/>
     </row>
     <row r="22" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="30" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="20"/>
@@ -5867,10 +5867,10 @@
       <c r="AT22" s="19"/>
     </row>
     <row r="23" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="33">
+      <c r="A23" s="31">
         <v>3.11</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="30" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="20"/>
@@ -5919,10 +5919,10 @@
       <c r="AT23" s="19"/>
     </row>
     <row r="24" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="33">
+      <c r="A24" s="31">
         <v>3.12</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="30" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="17"/>
@@ -5971,10 +5971,10 @@
       <c r="AT24" s="18"/>
     </row>
     <row r="25" spans="1:46" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="30" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="20"/>
@@ -6231,7 +6231,7 @@
       <c r="AT29" s="19"/>
     </row>
     <row r="30" spans="1:46" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="26" t="s">
         <v>88</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -6257,7 +6257,7 @@
       <c r="T30" s="19"/>
       <c r="U30" s="19"/>
       <c r="V30" s="19"/>
-      <c r="W30" s="30"/>
+      <c r="W30" s="28"/>
       <c r="X30" s="19"/>
       <c r="Y30" s="19"/>
       <c r="Z30" s="19"/>
@@ -6283,10 +6283,10 @@
       <c r="AT30" s="19"/>
     </row>
     <row r="31" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="31">
+      <c r="A31" s="29">
         <v>4.5</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="30" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="20"/>
@@ -6335,10 +6335,10 @@
       <c r="AT31" s="19"/>
     </row>
     <row r="32" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="31">
+      <c r="A32" s="29">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C32" s="20"/>
@@ -6387,10 +6387,10 @@
       <c r="AT32" s="19"/>
     </row>
     <row r="33" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="31">
+      <c r="A33" s="29">
         <v>4.7</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="30" t="s">
         <v>60</v>
       </c>
       <c r="C33" s="20"/>
@@ -6439,10 +6439,10 @@
       <c r="AT33" s="19"/>
     </row>
     <row r="34" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="31">
+      <c r="A34" s="29">
         <v>4.8</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="30" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="20"/>
@@ -6491,10 +6491,10 @@
       <c r="AT34" s="19"/>
     </row>
     <row r="35" spans="1:46" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="31">
+      <c r="A35" s="29">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="30" t="s">
         <v>62</v>
       </c>
       <c r="C35" s="20"/>
@@ -6699,7 +6699,7 @@
       <c r="A39" s="13">
         <v>5.4</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="30" t="s">
         <v>67</v>
       </c>
       <c r="C39" s="20"/>
@@ -6751,7 +6751,7 @@
       <c r="A40" s="13">
         <v>5.5</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="30" t="s">
         <v>68</v>
       </c>
       <c r="C40" s="20"/>
@@ -6803,7 +6803,7 @@
       <c r="A41" s="13">
         <v>5.6</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C41" s="20"/>
@@ -6855,7 +6855,7 @@
       <c r="A42" s="13">
         <v>5.7</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B42" s="30" t="s">
         <v>70</v>
       </c>
       <c r="C42" s="20"/>
@@ -6907,7 +6907,7 @@
       <c r="A43" s="13">
         <v>5.8</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="30" t="s">
         <v>71</v>
       </c>
       <c r="C43" s="20"/>
@@ -7060,7 +7060,7 @@
       <c r="AT45" s="19"/>
     </row>
     <row r="46" spans="1:46" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A46" s="28" t="s">
+      <c r="A46" s="26" t="s">
         <v>92</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -7092,7 +7092,7 @@
       <c r="AB46" s="19"/>
       <c r="AC46" s="19"/>
       <c r="AD46" s="19"/>
-      <c r="AE46" s="30"/>
+      <c r="AE46" s="28"/>
       <c r="AF46" s="19"/>
       <c r="AG46" s="19"/>
       <c r="AH46" s="19"/>
@@ -7113,7 +7113,7 @@
       <c r="A47" s="13">
         <v>6.3</v>
       </c>
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="30" t="s">
         <v>82</v>
       </c>
       <c r="C47" s="20"/>
@@ -7165,7 +7165,7 @@
       <c r="A48" s="13">
         <v>6.4</v>
       </c>
-      <c r="B48" s="32" t="s">
+      <c r="B48" s="30" t="s">
         <v>73</v>
       </c>
       <c r="C48" s="20"/>
@@ -7217,7 +7217,7 @@
       <c r="A49" s="13">
         <v>6.5</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="30" t="s">
         <v>74</v>
       </c>
       <c r="C49" s="20"/>
@@ -7269,7 +7269,7 @@
       <c r="A50" s="13">
         <v>6.6</v>
       </c>
-      <c r="B50" s="32" t="s">
+      <c r="B50" s="30" t="s">
         <v>91</v>
       </c>
       <c r="C50" s="20"/>
@@ -7354,240 +7354,240 @@
   <sheetData>
     <row r="1" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="39" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7652,236 +7652,236 @@
   <sheetData>
     <row r="1" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="44"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="45"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B5" s="45"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="45"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="47"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="45"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="47"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="45"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B8" s="45"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="47"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="45"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="50"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="48"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="44"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="42"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="47"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="45"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B13" s="45"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="45"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="47"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="45"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="47"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="45"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="47"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="45"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="50"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7910,232 +7910,232 @@
   <sheetData>
     <row r="1" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B3" s="42"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="44"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="45"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B5" s="45"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="45"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="47"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="45"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="47"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="45"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B8" s="45"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="47"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="45"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="50"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="48"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="44"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="42"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="47"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="45"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B13" s="45"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="45"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="47"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="45"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="47"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="45"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="47"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="45"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="50"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
update data validation in issue log
</commit_message>
<xml_diff>
--- a/01_doc/proj_plan/餐厅订餐系统_项目计划.xlsx
+++ b/01_doc/proj_plan/餐厅订餐系统_项目计划.xlsx
@@ -19,6 +19,7 @@
     <sheet name="Lengend" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1454,6 +1455,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1598,7 +1600,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2645,7 +2646,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2885,700 +2886,700 @@
   <sheetData>
     <row r="1" spans="2:13" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="54"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="56"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="57"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="56"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="57"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="56"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="57"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="54"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="56"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="57"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="56"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="57"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="56"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="57"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="57"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="59"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="60"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="61"/>
-      <c r="M14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="63"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="65"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="66"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="63"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="65"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="66"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="65"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="66"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="65"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="66"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="63"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="64"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="64"/>
-      <c r="M19" s="65"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="66"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="63"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="65"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="66"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="63"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="65"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="66"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="63"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="65"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="66"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="63"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="64"/>
-      <c r="M23" s="65"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="66"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="63"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="65"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="65"/>
+      <c r="M24" s="66"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="63"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="65"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="66"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="63"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="65"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="66"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="66"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="67"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="68"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="68"/>
+      <c r="M27" s="69"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="51" t="s">
+      <c r="B28" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="45"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="47"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="48"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="45"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="47"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="48"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="45"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="47"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="48"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="45"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="47"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="48"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="45"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="46"/>
-      <c r="M34" s="47"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="48"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="48"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="50"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="51"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="51"/>
-      <c r="M36" s="51"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="61" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="69"/>
-      <c r="L37" s="69"/>
-      <c r="M37" s="70"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="70"/>
+      <c r="M37" s="71"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="71"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="72"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="73"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="73"/>
+      <c r="M38" s="74"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="71"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="72"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="72"/>
-      <c r="M39" s="73"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="73"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="73"/>
+      <c r="M39" s="74"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="71"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
-      <c r="F40" s="72"/>
-      <c r="G40" s="72"/>
-      <c r="H40" s="72"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="72"/>
-      <c r="K40" s="72"/>
-      <c r="L40" s="72"/>
-      <c r="M40" s="73"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="73"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="73"/>
+      <c r="M40" s="74"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="74"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
-      <c r="M41" s="76"/>
+      <c r="B41" s="75"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="77"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
-      <c r="M43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="45"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="45"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
-      <c r="K44" s="46"/>
-      <c r="L44" s="46"/>
-      <c r="M44" s="47"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="47"/>
+      <c r="M44" s="48"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="45"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="47"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="47"/>
+      <c r="M45" s="48"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="47"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="47"/>
+      <c r="M46" s="48"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="45"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="46"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="46"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="46"/>
-      <c r="M47" s="47"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="47"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
+      <c r="M47" s="48"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="45"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="46"/>
-      <c r="H48" s="46"/>
-      <c r="I48" s="46"/>
-      <c r="J48" s="46"/>
-      <c r="K48" s="46"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="47"/>
+      <c r="B48" s="46"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="47"/>
+      <c r="J48" s="47"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="47"/>
+      <c r="M48" s="48"/>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="48"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="49"/>
-      <c r="I49" s="49"/>
-      <c r="J49" s="49"/>
-      <c r="K49" s="49"/>
-      <c r="L49" s="49"/>
-      <c r="M49" s="50"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="50"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="50"/>
+      <c r="M49" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3627,10 +3628,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
       <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
@@ -3645,10 +3646,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="77">
+      <c r="A3" s="78">
         <v>1</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="78" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="7">
@@ -3671,8 +3672,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="77"/>
-      <c r="B4" s="77"/>
+      <c r="A4" s="78"/>
+      <c r="B4" s="78"/>
       <c r="C4" s="7">
         <v>1.2</v>
       </c>
@@ -3693,8 +3694,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
+      <c r="A5" s="78"/>
+      <c r="B5" s="78"/>
       <c r="C5" s="7">
         <v>1.3</v>
       </c>
@@ -3715,8 +3716,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
       <c r="C6" s="7">
         <v>1.4</v>
       </c>
@@ -3737,10 +3738,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="79">
+      <c r="A7" s="80">
         <v>2</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="7">
@@ -3763,8 +3764,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="80"/>
-      <c r="B8" s="77"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="7">
         <v>2.2000000000000002</v>
       </c>
@@ -3785,8 +3786,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="81"/>
-      <c r="B9" s="77"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="7">
         <v>2.2999999999999998</v>
       </c>
@@ -3807,10 +3808,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="77">
+      <c r="A10" s="78">
         <v>3</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="78" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="9">
@@ -3833,8 +3834,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="77"/>
-      <c r="B11" s="77"/>
+      <c r="A11" s="78"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="9">
         <v>3.2</v>
       </c>
@@ -3855,8 +3856,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="77"/>
-      <c r="B12" s="77"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="9">
         <v>3.3</v>
       </c>
@@ -3877,8 +3878,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="77"/>
-      <c r="B13" s="77"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="9">
         <v>3.4</v>
       </c>
@@ -3899,8 +3900,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="77"/>
-      <c r="B14" s="77"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="9">
         <v>3.5</v>
       </c>
@@ -3921,8 +3922,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="77"/>
-      <c r="B15" s="77"/>
+      <c r="A15" s="78"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="9">
         <v>3.6</v>
       </c>
@@ -3943,8 +3944,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="77"/>
-      <c r="B16" s="77"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="9">
         <v>3.7</v>
       </c>
@@ -3965,8 +3966,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="77"/>
-      <c r="B17" s="77"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="9">
         <v>3.8</v>
       </c>
@@ -3987,8 +3988,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="77"/>
-      <c r="B18" s="77"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="9">
         <v>3.9</v>
       </c>
@@ -4009,8 +4010,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="78"/>
       <c r="C19" s="9" t="s">
         <v>51</v>
       </c>
@@ -4031,8 +4032,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="78"/>
       <c r="C20" s="9">
         <v>3.11</v>
       </c>
@@ -4053,8 +4054,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="78"/>
+      <c r="B21" s="78"/>
       <c r="C21" s="9">
         <v>3.12</v>
       </c>
@@ -4075,10 +4076,10 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="77">
+      <c r="A22" s="78">
         <v>4</v>
       </c>
-      <c r="B22" s="79" t="s">
+      <c r="B22" s="80" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="7">
@@ -4101,8 +4102,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23" s="77"/>
-      <c r="B23" s="80"/>
+      <c r="A23" s="78"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="7">
         <v>4.2</v>
       </c>
@@ -4123,8 +4124,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="77"/>
-      <c r="B24" s="80"/>
+      <c r="A24" s="78"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="7">
         <v>4.3</v>
       </c>
@@ -4145,8 +4146,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="77"/>
-      <c r="B25" s="80"/>
+      <c r="A25" s="78"/>
+      <c r="B25" s="81"/>
       <c r="C25" s="7">
         <v>4.4000000000000004</v>
       </c>
@@ -4167,8 +4168,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="77"/>
-      <c r="B26" s="80"/>
+      <c r="A26" s="78"/>
+      <c r="B26" s="81"/>
       <c r="C26" s="7">
         <v>4.5</v>
       </c>
@@ -4189,8 +4190,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A27" s="77"/>
-      <c r="B27" s="80"/>
+      <c r="A27" s="78"/>
+      <c r="B27" s="81"/>
       <c r="C27" s="7">
         <v>4.5999999999999996</v>
       </c>
@@ -4211,8 +4212,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="77"/>
-      <c r="B28" s="80"/>
+      <c r="A28" s="78"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="7">
         <v>4.7</v>
       </c>
@@ -4233,8 +4234,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="77"/>
-      <c r="B29" s="80"/>
+      <c r="A29" s="78"/>
+      <c r="B29" s="81"/>
       <c r="C29" s="7">
         <v>4.8</v>
       </c>
@@ -4255,10 +4256,10 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="77">
+      <c r="A30" s="78">
         <v>5</v>
       </c>
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="78" t="s">
         <v>63</v>
       </c>
       <c r="C30" s="7">
@@ -4281,8 +4282,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A31" s="77"/>
-      <c r="B31" s="77"/>
+      <c r="A31" s="78"/>
+      <c r="B31" s="78"/>
       <c r="C31" s="7">
         <v>5.2</v>
       </c>
@@ -4303,8 +4304,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="77"/>
-      <c r="B32" s="77"/>
+      <c r="A32" s="78"/>
+      <c r="B32" s="78"/>
       <c r="C32" s="7">
         <v>5.3</v>
       </c>
@@ -4325,8 +4326,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A33" s="77"/>
-      <c r="B33" s="77"/>
+      <c r="A33" s="78"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="7">
         <v>5.4</v>
       </c>
@@ -4347,8 +4348,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="77"/>
-      <c r="B34" s="77"/>
+      <c r="A34" s="78"/>
+      <c r="B34" s="78"/>
       <c r="C34" s="7">
         <v>5.5</v>
       </c>
@@ -4369,8 +4370,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A35" s="77"/>
-      <c r="B35" s="77"/>
+      <c r="A35" s="78"/>
+      <c r="B35" s="78"/>
       <c r="C35" s="7">
         <v>5.6</v>
       </c>
@@ -4391,8 +4392,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A36" s="77"/>
-      <c r="B36" s="77"/>
+      <c r="A36" s="78"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="7">
         <v>5.7</v>
       </c>
@@ -4413,10 +4414,10 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A37" s="77">
+      <c r="A37" s="78">
         <v>6</v>
       </c>
-      <c r="B37" s="77" t="s">
+      <c r="B37" s="78" t="s">
         <v>72</v>
       </c>
       <c r="C37" s="7">
@@ -4439,8 +4440,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A38" s="77"/>
-      <c r="B38" s="77"/>
+      <c r="A38" s="78"/>
+      <c r="B38" s="78"/>
       <c r="C38" s="7">
         <v>6.2</v>
       </c>
@@ -4461,8 +4462,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39" s="77"/>
-      <c r="B39" s="77"/>
+      <c r="A39" s="78"/>
+      <c r="B39" s="78"/>
       <c r="C39" s="7">
         <v>6.3</v>
       </c>
@@ -4483,8 +4484,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="77"/>
-      <c r="B40" s="77"/>
+      <c r="A40" s="78"/>
+      <c r="B40" s="78"/>
       <c r="C40" s="7">
         <v>6.4</v>
       </c>
@@ -4505,8 +4506,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
+      <c r="A41" s="78"/>
+      <c r="B41" s="78"/>
       <c r="C41" s="7">
         <v>6.5</v>
       </c>
@@ -4527,8 +4528,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A42" s="77"/>
-      <c r="B42" s="77"/>
+      <c r="A42" s="78"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="7">
         <v>6.6</v>
       </c>
@@ -4884,60 +4885,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="87"/>
-      <c r="B1" s="87"/>
-      <c r="C1" s="89" t="s">
+      <c r="A1" s="88"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="82" t="s">
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="83"/>
-      <c r="AB1" s="83"/>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
-      <c r="AG1" s="83"/>
-      <c r="AH1" s="83"/>
-      <c r="AI1" s="83"/>
-      <c r="AJ1" s="83"/>
-      <c r="AK1" s="83"/>
-      <c r="AL1" s="83"/>
-      <c r="AM1" s="83"/>
-      <c r="AN1" s="83"/>
-      <c r="AO1" s="83"/>
-      <c r="AP1" s="83"/>
-      <c r="AQ1" s="83"/>
-      <c r="AR1" s="83"/>
-      <c r="AS1" s="83"/>
-      <c r="AT1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
+      <c r="AG1" s="84"/>
+      <c r="AH1" s="84"/>
+      <c r="AI1" s="84"/>
+      <c r="AJ1" s="84"/>
+      <c r="AK1" s="84"/>
+      <c r="AL1" s="84"/>
+      <c r="AM1" s="84"/>
+      <c r="AN1" s="84"/>
+      <c r="AO1" s="84"/>
+      <c r="AP1" s="84"/>
+      <c r="AQ1" s="84"/>
+      <c r="AR1" s="84"/>
+      <c r="AS1" s="84"/>
+      <c r="AT1" s="85"/>
     </row>
     <row r="2" spans="1:58" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="88"/>
-      <c r="B2" s="88"/>
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
       <c r="C2" s="16">
         <v>18</v>
       </c>
@@ -5090,9 +5091,9 @@
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -7899,7 +7900,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7964,7 +7965,7 @@
       <c r="I2" s="32"/>
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
-      <c r="L2" s="90"/>
+      <c r="L2" s="42"/>
     </row>
     <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="32"/>
@@ -7978,7 +7979,7 @@
       <c r="I3" s="32"/>
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
-      <c r="L3" s="90"/>
+      <c r="L3" s="42"/>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="32"/>
@@ -7992,7 +7993,7 @@
       <c r="I4" s="32"/>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
-      <c r="L4" s="90"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="32"/>
@@ -8006,7 +8007,7 @@
       <c r="I5" s="32"/>
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
-      <c r="L5" s="90"/>
+      <c r="L5" s="42"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="32"/>
@@ -8020,7 +8021,7 @@
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
-      <c r="L6" s="90"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="32"/>
@@ -8034,7 +8035,7 @@
       <c r="I7" s="32"/>
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
-      <c r="L7" s="90"/>
+      <c r="L7" s="42"/>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="32"/>
@@ -8048,7 +8049,7 @@
       <c r="I8" s="32"/>
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
-      <c r="L8" s="90"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="32"/>
@@ -8062,7 +8063,7 @@
       <c r="I9" s="32"/>
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
-      <c r="L9" s="90"/>
+      <c r="L9" s="42"/>
     </row>
     <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="32"/>
@@ -8076,7 +8077,7 @@
       <c r="I10" s="32"/>
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
-      <c r="L10" s="90"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="32"/>
@@ -8090,7 +8091,7 @@
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
-      <c r="L11" s="90"/>
+      <c r="L11" s="42"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="32"/>
@@ -8104,7 +8105,7 @@
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
-      <c r="L12" s="90"/>
+      <c r="L12" s="42"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
@@ -8118,7 +8119,7 @@
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
-      <c r="L13" s="90"/>
+      <c r="L13" s="42"/>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
@@ -8132,7 +8133,7 @@
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
-      <c r="L14" s="90"/>
+      <c r="L14" s="42"/>
     </row>
     <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="32"/>
@@ -8146,7 +8147,7 @@
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
-      <c r="L15" s="90"/>
+      <c r="L15" s="42"/>
     </row>
     <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="32"/>
@@ -8160,7 +8161,7 @@
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
-      <c r="L16" s="90"/>
+      <c r="L16" s="42"/>
     </row>
     <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="32"/>
@@ -8174,7 +8175,7 @@
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
-      <c r="L17" s="90"/>
+      <c r="L17" s="42"/>
     </row>
     <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="32"/>
@@ -8188,7 +8189,7 @@
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
-      <c r="L18" s="90"/>
+      <c r="L18" s="42"/>
     </row>
     <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="32"/>
@@ -8202,7 +8203,7 @@
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
-      <c r="L19" s="90"/>
+      <c r="L19" s="42"/>
     </row>
     <row r="20" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="32"/>
@@ -8216,7 +8217,7 @@
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
-      <c r="L20" s="90"/>
+      <c r="L20" s="42"/>
     </row>
     <row r="21" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="32"/>
@@ -8230,7 +8231,7 @@
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
-      <c r="L21" s="90"/>
+      <c r="L21" s="42"/>
     </row>
     <row r="22" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="32"/>
@@ -8244,13 +8245,19 @@
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
-      <c r="L22" s="90"/>
+      <c r="L22" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lengend!$B$12:$B$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lengend!$G$12:$G$15</xm:f>
@@ -8259,21 +8266,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[1]Lengend!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J22</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>Lengend!$A$7:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>I1:I1048576 G1:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lengend!$B$12:$B$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>G1:G1048576 I1:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8297,306 +8292,306 @@
   <sheetData>
     <row r="1" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="45"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="48"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B5" s="45"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="48"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="47"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="48"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="47"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="48"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B8" s="45"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="47"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="48"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="50"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="51"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="45"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="47"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="48"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B13" s="45"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="48"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="47"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="48"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="47"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="48"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="47"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="48"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="47"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="48"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="47"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="48"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B19" s="45"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="47"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="48"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="47"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="48"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="47"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="48"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="50"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -8625,232 +8620,232 @@
   <sheetData>
     <row r="1" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B3" s="42"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="44"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="45"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="48"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B5" s="45"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="48"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="47"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="48"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="47"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="48"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B8" s="45"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="47"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="48"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="50"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="51"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="44"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="45"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="47"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="48"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B13" s="45"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="48"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="47"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="48"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="47"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="48"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="47"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="48"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="50"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
update aaron's progress on WS development
</commit_message>
<xml_diff>
--- a/01_doc/proj_plan/餐厅订餐系统_项目计划.xlsx
+++ b/01_doc/proj_plan/餐厅订餐系统_项目计划.xlsx
@@ -1756,7 +1756,7 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1808,6 +1808,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1993,7 +1999,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2073,6 +2079,19 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2178,6 +2197,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2185,9 +2207,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2229,19 +2248,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3791,232 +3798,232 @@
   <sheetData>
     <row r="1" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B3" s="51"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="53"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="56"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="61"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="56"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="61"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="56"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="61"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="56"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="61"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="56"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="61"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="59"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="64"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="53"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="58"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="56"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="61"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
-      <c r="M13" s="56"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="61"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="56"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="61"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="56"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="61"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="56"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="61"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="57"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="59"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4274,700 +4281,700 @@
   <sheetData>
     <row r="1" spans="2:13" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="62"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="67"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="63"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="65"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="70"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="63"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="65"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="70"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="63"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="70"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="62"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="67"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="63"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="65"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="70"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="63"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="65"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="70"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="63"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="65"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="70"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="66"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="68"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="73"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="74" t="s">
         <v>171</v>
       </c>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="70"/>
-      <c r="M14" s="71"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="76"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="72"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="74"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="79"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="72"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="74"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="79"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="72"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="74"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="78"/>
+      <c r="L17" s="78"/>
+      <c r="M17" s="79"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="72"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="74"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="78"/>
+      <c r="L18" s="78"/>
+      <c r="M18" s="79"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="72"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="74"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="78"/>
+      <c r="M19" s="79"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="72"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="74"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="78"/>
+      <c r="M20" s="79"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="72"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="74"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="78"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="78"/>
+      <c r="L21" s="78"/>
+      <c r="M21" s="79"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="72"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="74"/>
+      <c r="B22" s="77"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="79"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="72"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="74"/>
+      <c r="B23" s="77"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="78"/>
+      <c r="L23" s="78"/>
+      <c r="M23" s="79"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="72"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
-      <c r="M24" s="74"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="78"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="78"/>
+      <c r="L24" s="78"/>
+      <c r="M24" s="79"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="72"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="74"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="79"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="72"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="73"/>
-      <c r="M26" s="74"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="79"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="75"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="76"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="76"/>
-      <c r="M27" s="77"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="81"/>
+      <c r="J27" s="81"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="82"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="60"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="65"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="53"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="57"/>
+      <c r="M29" s="58"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="54"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="55"/>
-      <c r="M30" s="56"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="61"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="54"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="56"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="61"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="54"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="55"/>
-      <c r="M32" s="56"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="61"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="54"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="55"/>
-      <c r="M33" s="56"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="61"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="54"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
-      <c r="L34" s="55"/>
-      <c r="M34" s="56"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="61"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="57"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="59"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="63"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="64"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="60"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="60"/>
-      <c r="I36" s="60"/>
-      <c r="J36" s="60"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="60"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="65"/>
+      <c r="L36" s="65"/>
+      <c r="M36" s="65"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="69" t="s">
+      <c r="B37" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="78"/>
-      <c r="J37" s="78"/>
-      <c r="K37" s="78"/>
-      <c r="L37" s="78"/>
-      <c r="M37" s="79"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="83"/>
+      <c r="M37" s="84"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="80"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
-      <c r="G38" s="81"/>
-      <c r="H38" s="81"/>
-      <c r="I38" s="81"/>
-      <c r="J38" s="81"/>
-      <c r="K38" s="81"/>
-      <c r="L38" s="81"/>
-      <c r="M38" s="82"/>
+      <c r="B38" s="85"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="86"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="86"/>
+      <c r="J38" s="86"/>
+      <c r="K38" s="86"/>
+      <c r="L38" s="86"/>
+      <c r="M38" s="87"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="80"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="81"/>
-      <c r="K39" s="81"/>
-      <c r="L39" s="81"/>
-      <c r="M39" s="82"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="86"/>
+      <c r="I39" s="86"/>
+      <c r="J39" s="86"/>
+      <c r="K39" s="86"/>
+      <c r="L39" s="86"/>
+      <c r="M39" s="87"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="80"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="81"/>
-      <c r="J40" s="81"/>
-      <c r="K40" s="81"/>
-      <c r="L40" s="81"/>
-      <c r="M40" s="82"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="86"/>
+      <c r="H40" s="86"/>
+      <c r="I40" s="86"/>
+      <c r="J40" s="86"/>
+      <c r="K40" s="86"/>
+      <c r="L40" s="86"/>
+      <c r="M40" s="87"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="83"/>
-      <c r="C41" s="84"/>
-      <c r="D41" s="84"/>
-      <c r="E41" s="84"/>
-      <c r="F41" s="84"/>
-      <c r="G41" s="84"/>
-      <c r="H41" s="84"/>
-      <c r="I41" s="84"/>
-      <c r="J41" s="84"/>
-      <c r="K41" s="84"/>
-      <c r="L41" s="84"/>
-      <c r="M41" s="85"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="89"/>
+      <c r="I41" s="89"/>
+      <c r="J41" s="89"/>
+      <c r="K41" s="89"/>
+      <c r="L41" s="89"/>
+      <c r="M41" s="90"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="60" t="s">
+      <c r="B42" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
-      <c r="H42" s="60"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="60"/>
-      <c r="L42" s="60"/>
-      <c r="M42" s="60"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="65"/>
+      <c r="J42" s="65"/>
+      <c r="K42" s="65"/>
+      <c r="L42" s="65"/>
+      <c r="M42" s="65"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="51" t="s">
+      <c r="B43" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="52"/>
-      <c r="I43" s="52"/>
-      <c r="J43" s="52"/>
-      <c r="K43" s="52"/>
-      <c r="L43" s="52"/>
-      <c r="M43" s="53"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="57"/>
+      <c r="M43" s="58"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="54"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="55"/>
-      <c r="M44" s="56"/>
+      <c r="B44" s="59"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="60"/>
+      <c r="I44" s="60"/>
+      <c r="J44" s="60"/>
+      <c r="K44" s="60"/>
+      <c r="L44" s="60"/>
+      <c r="M44" s="61"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="54"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="55"/>
-      <c r="M45" s="56"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="60"/>
+      <c r="J45" s="60"/>
+      <c r="K45" s="60"/>
+      <c r="L45" s="60"/>
+      <c r="M45" s="61"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="54"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
-      <c r="L46" s="55"/>
-      <c r="M46" s="56"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="60"/>
+      <c r="J46" s="60"/>
+      <c r="K46" s="60"/>
+      <c r="L46" s="60"/>
+      <c r="M46" s="61"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="54"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="55"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="55"/>
-      <c r="L47" s="55"/>
-      <c r="M47" s="56"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="60"/>
+      <c r="K47" s="60"/>
+      <c r="L47" s="60"/>
+      <c r="M47" s="61"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="54"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="55"/>
-      <c r="L48" s="55"/>
-      <c r="M48" s="56"/>
+      <c r="B48" s="59"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="60"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="60"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="60"/>
+      <c r="L48" s="60"/>
+      <c r="M48" s="61"/>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="57"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="58"/>
-      <c r="M49" s="59"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="63"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="63"/>
+      <c r="J49" s="63"/>
+      <c r="K49" s="63"/>
+      <c r="L49" s="63"/>
+      <c r="M49" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -5016,10 +5023,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="86"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
       <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
@@ -5034,10 +5041,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="89">
+      <c r="A3" s="91">
         <v>1</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="91" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="7">
@@ -5060,8 +5067,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="89"/>
-      <c r="B4" s="89"/>
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
       <c r="C4" s="7">
         <v>1.2</v>
       </c>
@@ -5082,8 +5089,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="89"/>
-      <c r="B5" s="89"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="91"/>
       <c r="C5" s="7">
         <v>1.3</v>
       </c>
@@ -5104,8 +5111,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="89"/>
-      <c r="B6" s="89"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="91"/>
       <c r="C6" s="7">
         <v>1.4</v>
       </c>
@@ -5126,10 +5133,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="87">
+      <c r="A7" s="93">
         <v>2</v>
       </c>
-      <c r="B7" s="89" t="s">
+      <c r="B7" s="91" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="7">
@@ -5152,8 +5159,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="88"/>
-      <c r="B8" s="89"/>
+      <c r="A8" s="94"/>
+      <c r="B8" s="91"/>
       <c r="C8" s="7">
         <v>2.2000000000000002</v>
       </c>
@@ -5174,8 +5181,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="90"/>
-      <c r="B9" s="89"/>
+      <c r="A9" s="95"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="7">
         <v>2.2999999999999998</v>
       </c>
@@ -5196,10 +5203,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="89">
+      <c r="A10" s="91">
         <v>3</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="91" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="9">
@@ -5222,8 +5229,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="89"/>
-      <c r="B11" s="89"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="9">
         <v>3.2</v>
       </c>
@@ -5244,8 +5251,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="89"/>
-      <c r="B12" s="89"/>
+      <c r="A12" s="91"/>
+      <c r="B12" s="91"/>
       <c r="C12" s="9">
         <v>3.3</v>
       </c>
@@ -5266,8 +5273,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="89"/>
-      <c r="B13" s="89"/>
+      <c r="A13" s="91"/>
+      <c r="B13" s="91"/>
       <c r="C13" s="9">
         <v>3.4</v>
       </c>
@@ -5288,8 +5295,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="89"/>
-      <c r="B14" s="89"/>
+      <c r="A14" s="91"/>
+      <c r="B14" s="91"/>
       <c r="C14" s="9">
         <v>3.5</v>
       </c>
@@ -5310,8 +5317,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="89"/>
-      <c r="B15" s="89"/>
+      <c r="A15" s="91"/>
+      <c r="B15" s="91"/>
       <c r="C15" s="9">
         <v>3.6</v>
       </c>
@@ -5332,8 +5339,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="89"/>
-      <c r="B16" s="89"/>
+      <c r="A16" s="91"/>
+      <c r="B16" s="91"/>
       <c r="C16" s="9">
         <v>3.7</v>
       </c>
@@ -5354,8 +5361,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="89"/>
-      <c r="B17" s="89"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="91"/>
       <c r="C17" s="9">
         <v>3.8</v>
       </c>
@@ -5376,8 +5383,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="89"/>
-      <c r="B18" s="89"/>
+      <c r="A18" s="91"/>
+      <c r="B18" s="91"/>
       <c r="C18" s="9">
         <v>3.9</v>
       </c>
@@ -5398,8 +5405,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="89"/>
-      <c r="B19" s="89"/>
+      <c r="A19" s="91"/>
+      <c r="B19" s="91"/>
       <c r="C19" s="9" t="s">
         <v>48</v>
       </c>
@@ -5420,10 +5427,10 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="89">
+      <c r="A20" s="91">
         <v>4</v>
       </c>
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="93" t="s">
         <v>50</v>
       </c>
       <c r="C20" s="7">
@@ -5446,8 +5453,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="89"/>
-      <c r="B21" s="88"/>
+      <c r="A21" s="91"/>
+      <c r="B21" s="94"/>
       <c r="C21" s="7">
         <v>4.2</v>
       </c>
@@ -5468,8 +5475,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="89"/>
-      <c r="B22" s="88"/>
+      <c r="A22" s="91"/>
+      <c r="B22" s="94"/>
       <c r="C22" s="7">
         <v>4.3</v>
       </c>
@@ -5490,8 +5497,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23" s="89"/>
-      <c r="B23" s="88"/>
+      <c r="A23" s="91"/>
+      <c r="B23" s="94"/>
       <c r="C23" s="7">
         <v>4.4000000000000004</v>
       </c>
@@ -5512,8 +5519,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="89"/>
-      <c r="B24" s="88"/>
+      <c r="A24" s="91"/>
+      <c r="B24" s="94"/>
       <c r="C24" s="7">
         <v>4.5</v>
       </c>
@@ -5534,8 +5541,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="89"/>
-      <c r="B25" s="88"/>
+      <c r="A25" s="91"/>
+      <c r="B25" s="94"/>
       <c r="C25" s="7">
         <v>4.5999999999999996</v>
       </c>
@@ -5556,10 +5563,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="89">
+      <c r="A26" s="91">
         <v>5</v>
       </c>
-      <c r="B26" s="89" t="s">
+      <c r="B26" s="91" t="s">
         <v>57</v>
       </c>
       <c r="C26" s="7">
@@ -5582,8 +5589,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A27" s="89"/>
-      <c r="B27" s="89"/>
+      <c r="A27" s="91"/>
+      <c r="B27" s="91"/>
       <c r="C27" s="7">
         <v>5.2</v>
       </c>
@@ -5604,8 +5611,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="89"/>
-      <c r="B28" s="89"/>
+      <c r="A28" s="91"/>
+      <c r="B28" s="91"/>
       <c r="C28" s="7">
         <v>5.3</v>
       </c>
@@ -5626,8 +5633,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="89"/>
-      <c r="B29" s="89"/>
+      <c r="A29" s="91"/>
+      <c r="B29" s="91"/>
       <c r="C29" s="7">
         <v>5.4</v>
       </c>
@@ -5648,8 +5655,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="89"/>
-      <c r="B30" s="89"/>
+      <c r="A30" s="91"/>
+      <c r="B30" s="91"/>
       <c r="C30" s="7">
         <v>5.5</v>
       </c>
@@ -5670,10 +5677,10 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A31" s="89">
+      <c r="A31" s="91">
         <v>6</v>
       </c>
-      <c r="B31" s="89" t="s">
+      <c r="B31" s="91" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="7">
@@ -5696,8 +5703,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="89"/>
-      <c r="B32" s="89"/>
+      <c r="A32" s="91"/>
+      <c r="B32" s="91"/>
       <c r="C32" s="7">
         <v>6.2</v>
       </c>
@@ -5718,8 +5725,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A33" s="89"/>
-      <c r="B33" s="89"/>
+      <c r="A33" s="91"/>
+      <c r="B33" s="91"/>
       <c r="C33" s="7">
         <v>6.3</v>
       </c>
@@ -5740,8 +5747,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="89"/>
-      <c r="B34" s="89"/>
+      <c r="A34" s="91"/>
+      <c r="B34" s="91"/>
       <c r="C34" s="7">
         <v>6.4</v>
       </c>
@@ -5762,8 +5769,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A35" s="89"/>
-      <c r="B35" s="89"/>
+      <c r="A35" s="91"/>
+      <c r="B35" s="91"/>
       <c r="C35" s="7">
         <v>6.5</v>
       </c>
@@ -5784,8 +5791,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A36" s="89"/>
-      <c r="B36" s="89"/>
+      <c r="A36" s="91"/>
+      <c r="B36" s="91"/>
       <c r="C36" s="7">
         <v>6.6</v>
       </c>
@@ -5806,10 +5813,10 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A37" s="89">
+      <c r="A37" s="91">
         <v>7</v>
       </c>
-      <c r="B37" s="89" t="s">
+      <c r="B37" s="91" t="s">
         <v>154</v>
       </c>
       <c r="C37" s="7">
@@ -5832,8 +5839,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A38" s="89"/>
-      <c r="B38" s="89"/>
+      <c r="A38" s="91"/>
+      <c r="B38" s="91"/>
       <c r="C38" s="7">
         <v>7.2</v>
       </c>
@@ -5854,8 +5861,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39" s="89"/>
-      <c r="B39" s="89"/>
+      <c r="A39" s="91"/>
+      <c r="B39" s="91"/>
       <c r="C39" s="7">
         <v>7.3</v>
       </c>
@@ -5876,8 +5883,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="89"/>
-      <c r="B40" s="89"/>
+      <c r="A40" s="91"/>
+      <c r="B40" s="91"/>
       <c r="C40" s="7">
         <v>7.4</v>
       </c>
@@ -5898,8 +5905,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A41" s="89"/>
-      <c r="B41" s="89"/>
+      <c r="A41" s="91"/>
+      <c r="B41" s="91"/>
       <c r="C41" s="7">
         <v>7.5</v>
       </c>
@@ -5921,11 +5928,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="A20:A25"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="B20:B25"/>
     <mergeCell ref="B26:B30"/>
@@ -5936,6 +5938,11 @@
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B19"/>
     <mergeCell ref="A10:A19"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="A20:A25"/>
   </mergeCells>
   <conditionalFormatting sqref="E3 E4:H30">
     <cfRule type="cellIs" dxfId="159" priority="217" operator="equal">
@@ -6537,60 +6544,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="96"/>
-      <c r="B1" s="96"/>
-      <c r="C1" s="98" t="s">
+      <c r="A1" s="101"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="91" t="s">
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
-      <c r="W1" s="92"/>
-      <c r="X1" s="92"/>
-      <c r="Y1" s="92"/>
-      <c r="Z1" s="92"/>
-      <c r="AA1" s="92"/>
-      <c r="AB1" s="92"/>
-      <c r="AC1" s="92"/>
-      <c r="AD1" s="92"/>
-      <c r="AE1" s="92"/>
-      <c r="AF1" s="92"/>
-      <c r="AG1" s="92"/>
-      <c r="AH1" s="92"/>
-      <c r="AI1" s="92"/>
-      <c r="AJ1" s="92"/>
-      <c r="AK1" s="92"/>
-      <c r="AL1" s="92"/>
-      <c r="AM1" s="92"/>
-      <c r="AN1" s="92"/>
-      <c r="AO1" s="92"/>
-      <c r="AP1" s="92"/>
-      <c r="AQ1" s="92"/>
-      <c r="AR1" s="92"/>
-      <c r="AS1" s="92"/>
-      <c r="AT1" s="93"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="97"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="97"/>
+      <c r="X1" s="97"/>
+      <c r="Y1" s="97"/>
+      <c r="Z1" s="97"/>
+      <c r="AA1" s="97"/>
+      <c r="AB1" s="97"/>
+      <c r="AC1" s="97"/>
+      <c r="AD1" s="97"/>
+      <c r="AE1" s="97"/>
+      <c r="AF1" s="97"/>
+      <c r="AG1" s="97"/>
+      <c r="AH1" s="97"/>
+      <c r="AI1" s="97"/>
+      <c r="AJ1" s="97"/>
+      <c r="AK1" s="97"/>
+      <c r="AL1" s="97"/>
+      <c r="AM1" s="97"/>
+      <c r="AN1" s="97"/>
+      <c r="AO1" s="97"/>
+      <c r="AP1" s="97"/>
+      <c r="AQ1" s="97"/>
+      <c r="AR1" s="97"/>
+      <c r="AS1" s="97"/>
+      <c r="AT1" s="98"/>
     </row>
     <row r="2" spans="1:58" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="97"/>
-      <c r="B2" s="97"/>
+      <c r="A2" s="102"/>
+      <c r="B2" s="102"/>
       <c r="C2" s="16">
         <v>18</v>
       </c>
@@ -6743,9 +6750,9 @@
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -9261,7 +9268,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE23" sqref="AE23"/>
+      <selection pane="bottomRight" activeCell="N10" sqref="N10:P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9277,361 +9284,361 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:82" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="106" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="102" t="s">
+      <c r="B1" s="106"/>
+      <c r="C1" s="107" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="99" t="s">
+      <c r="D1" s="104" t="s">
         <v>172</v>
       </c>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
-      <c r="W1" s="99"/>
-      <c r="X1" s="99"/>
-      <c r="Y1" s="99"/>
-      <c r="Z1" s="99"/>
-      <c r="AA1" s="100" t="s">
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104"/>
+      <c r="S1" s="104"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="104"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="104"/>
+      <c r="X1" s="104"/>
+      <c r="Y1" s="104"/>
+      <c r="Z1" s="104"/>
+      <c r="AA1" s="105" t="s">
         <v>173</v>
       </c>
-      <c r="AB1" s="100"/>
-      <c r="AC1" s="100"/>
-      <c r="AD1" s="100"/>
-      <c r="AE1" s="100"/>
-      <c r="AF1" s="100"/>
-      <c r="AG1" s="100"/>
-      <c r="AH1" s="100"/>
-      <c r="AI1" s="100"/>
-      <c r="AJ1" s="100"/>
-      <c r="AK1" s="100"/>
-      <c r="AL1" s="100"/>
-      <c r="AM1" s="100"/>
-      <c r="AN1" s="100"/>
-      <c r="AO1" s="100"/>
-      <c r="AP1" s="100"/>
-      <c r="AQ1" s="100"/>
-      <c r="AR1" s="100"/>
-      <c r="AS1" s="100"/>
-      <c r="AT1" s="100"/>
-      <c r="AU1" s="100"/>
-      <c r="AV1" s="100"/>
-      <c r="AW1" s="100"/>
-      <c r="AX1" s="100"/>
-      <c r="AY1" s="100"/>
-      <c r="AZ1" s="100"/>
-      <c r="BA1" s="100"/>
-      <c r="BB1" s="100"/>
-      <c r="BC1" s="100"/>
-      <c r="BD1" s="100"/>
-      <c r="BE1" s="100" t="s">
+      <c r="AB1" s="105"/>
+      <c r="AC1" s="105"/>
+      <c r="AD1" s="105"/>
+      <c r="AE1" s="105"/>
+      <c r="AF1" s="105"/>
+      <c r="AG1" s="105"/>
+      <c r="AH1" s="105"/>
+      <c r="AI1" s="105"/>
+      <c r="AJ1" s="105"/>
+      <c r="AK1" s="105"/>
+      <c r="AL1" s="105"/>
+      <c r="AM1" s="105"/>
+      <c r="AN1" s="105"/>
+      <c r="AO1" s="105"/>
+      <c r="AP1" s="105"/>
+      <c r="AQ1" s="105"/>
+      <c r="AR1" s="105"/>
+      <c r="AS1" s="105"/>
+      <c r="AT1" s="105"/>
+      <c r="AU1" s="105"/>
+      <c r="AV1" s="105"/>
+      <c r="AW1" s="105"/>
+      <c r="AX1" s="105"/>
+      <c r="AY1" s="105"/>
+      <c r="AZ1" s="105"/>
+      <c r="BA1" s="105"/>
+      <c r="BB1" s="105"/>
+      <c r="BC1" s="105"/>
+      <c r="BD1" s="105"/>
+      <c r="BE1" s="105" t="s">
         <v>188</v>
       </c>
-      <c r="BF1" s="100"/>
-      <c r="BG1" s="100"/>
-      <c r="BH1" s="100"/>
-      <c r="BI1" s="100"/>
-      <c r="BJ1" s="100"/>
-      <c r="BK1" s="100"/>
-      <c r="BL1" s="100"/>
-      <c r="BM1" s="100"/>
-      <c r="BN1" s="100"/>
-      <c r="BO1" s="100"/>
-      <c r="BP1" s="100"/>
-      <c r="BQ1" s="100"/>
-      <c r="BR1" s="100"/>
-    </row>
-    <row r="2" spans="1:82" s="107" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="101"/>
-      <c r="B2" s="101"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="103">
+      <c r="BF1" s="105"/>
+      <c r="BG1" s="105"/>
+      <c r="BH1" s="105"/>
+      <c r="BI1" s="105"/>
+      <c r="BJ1" s="105"/>
+      <c r="BK1" s="105"/>
+      <c r="BL1" s="105"/>
+      <c r="BM1" s="105"/>
+      <c r="BN1" s="105"/>
+      <c r="BO1" s="105"/>
+      <c r="BP1" s="105"/>
+      <c r="BQ1" s="105"/>
+      <c r="BR1" s="105"/>
+    </row>
+    <row r="2" spans="1:82" s="55" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="106"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="51">
         <v>41707</v>
       </c>
-      <c r="E2" s="104">
+      <c r="E2" s="52">
         <f>DATE(YEAR(D2),MONTH(D2),DAY(D2)+1)</f>
         <v>41708</v>
       </c>
-      <c r="F2" s="104">
+      <c r="F2" s="52">
         <f t="shared" ref="F2:BO2" si="0">DATE(YEAR(E2),MONTH(E2),DAY(E2)+1)</f>
         <v>41709</v>
       </c>
-      <c r="G2" s="104">
+      <c r="G2" s="52">
         <f t="shared" si="0"/>
         <v>41710</v>
       </c>
-      <c r="H2" s="104">
+      <c r="H2" s="52">
         <f t="shared" si="0"/>
         <v>41711</v>
       </c>
-      <c r="I2" s="104">
+      <c r="I2" s="52">
         <f t="shared" si="0"/>
         <v>41712</v>
       </c>
-      <c r="J2" s="104">
+      <c r="J2" s="52">
         <f t="shared" si="0"/>
         <v>41713</v>
       </c>
-      <c r="K2" s="104">
+      <c r="K2" s="52">
         <f t="shared" si="0"/>
         <v>41714</v>
       </c>
-      <c r="L2" s="104">
+      <c r="L2" s="52">
         <f t="shared" si="0"/>
         <v>41715</v>
       </c>
-      <c r="M2" s="104">
+      <c r="M2" s="52">
         <f t="shared" si="0"/>
         <v>41716</v>
       </c>
-      <c r="N2" s="104">
+      <c r="N2" s="52">
         <f t="shared" si="0"/>
         <v>41717</v>
       </c>
-      <c r="O2" s="104">
+      <c r="O2" s="52">
         <f t="shared" si="0"/>
         <v>41718</v>
       </c>
-      <c r="P2" s="104">
+      <c r="P2" s="52">
         <f t="shared" si="0"/>
         <v>41719</v>
       </c>
-      <c r="Q2" s="104">
+      <c r="Q2" s="52">
         <f t="shared" si="0"/>
         <v>41720</v>
       </c>
-      <c r="R2" s="104">
+      <c r="R2" s="52">
         <f t="shared" si="0"/>
         <v>41721</v>
       </c>
-      <c r="S2" s="104">
+      <c r="S2" s="52">
         <f t="shared" si="0"/>
         <v>41722</v>
       </c>
-      <c r="T2" s="104">
+      <c r="T2" s="52">
         <f t="shared" si="0"/>
         <v>41723</v>
       </c>
-      <c r="U2" s="104">
+      <c r="U2" s="52">
         <f t="shared" si="0"/>
         <v>41724</v>
       </c>
-      <c r="V2" s="104">
+      <c r="V2" s="52">
         <f t="shared" si="0"/>
         <v>41725</v>
       </c>
-      <c r="W2" s="104">
+      <c r="W2" s="52">
         <f t="shared" si="0"/>
         <v>41726</v>
       </c>
-      <c r="X2" s="104">
+      <c r="X2" s="52">
         <f t="shared" si="0"/>
         <v>41727</v>
       </c>
-      <c r="Y2" s="104">
+      <c r="Y2" s="52">
         <f t="shared" si="0"/>
         <v>41728</v>
       </c>
-      <c r="Z2" s="104">
+      <c r="Z2" s="52">
         <f t="shared" si="0"/>
         <v>41729</v>
       </c>
-      <c r="AA2" s="104">
+      <c r="AA2" s="52">
         <f t="shared" si="0"/>
         <v>41730</v>
       </c>
-      <c r="AB2" s="104">
+      <c r="AB2" s="52">
         <f t="shared" si="0"/>
         <v>41731</v>
       </c>
-      <c r="AC2" s="104">
+      <c r="AC2" s="52">
         <f t="shared" si="0"/>
         <v>41732</v>
       </c>
-      <c r="AD2" s="104">
+      <c r="AD2" s="52">
         <f t="shared" si="0"/>
         <v>41733</v>
       </c>
-      <c r="AE2" s="104">
+      <c r="AE2" s="52">
         <f t="shared" si="0"/>
         <v>41734</v>
       </c>
-      <c r="AF2" s="104">
+      <c r="AF2" s="52">
         <f t="shared" si="0"/>
         <v>41735</v>
       </c>
-      <c r="AG2" s="104">
+      <c r="AG2" s="52">
         <f t="shared" si="0"/>
         <v>41736</v>
       </c>
-      <c r="AH2" s="104">
+      <c r="AH2" s="52">
         <f t="shared" si="0"/>
         <v>41737</v>
       </c>
-      <c r="AI2" s="104">
+      <c r="AI2" s="52">
         <f t="shared" si="0"/>
         <v>41738</v>
       </c>
-      <c r="AJ2" s="104">
+      <c r="AJ2" s="52">
         <f t="shared" si="0"/>
         <v>41739</v>
       </c>
-      <c r="AK2" s="104">
+      <c r="AK2" s="52">
         <f t="shared" si="0"/>
         <v>41740</v>
       </c>
-      <c r="AL2" s="104">
+      <c r="AL2" s="52">
         <f t="shared" si="0"/>
         <v>41741</v>
       </c>
-      <c r="AM2" s="104">
+      <c r="AM2" s="52">
         <f t="shared" si="0"/>
         <v>41742</v>
       </c>
-      <c r="AN2" s="104">
+      <c r="AN2" s="52">
         <f t="shared" si="0"/>
         <v>41743</v>
       </c>
-      <c r="AO2" s="104">
+      <c r="AO2" s="52">
         <f t="shared" si="0"/>
         <v>41744</v>
       </c>
-      <c r="AP2" s="104">
+      <c r="AP2" s="52">
         <f t="shared" si="0"/>
         <v>41745</v>
       </c>
-      <c r="AQ2" s="104">
+      <c r="AQ2" s="52">
         <f t="shared" si="0"/>
         <v>41746</v>
       </c>
-      <c r="AR2" s="104">
+      <c r="AR2" s="52">
         <f t="shared" si="0"/>
         <v>41747</v>
       </c>
-      <c r="AS2" s="104">
+      <c r="AS2" s="52">
         <f t="shared" si="0"/>
         <v>41748</v>
       </c>
-      <c r="AT2" s="104">
+      <c r="AT2" s="52">
         <f t="shared" si="0"/>
         <v>41749</v>
       </c>
-      <c r="AU2" s="104">
+      <c r="AU2" s="52">
         <f t="shared" si="0"/>
         <v>41750</v>
       </c>
-      <c r="AV2" s="104">
+      <c r="AV2" s="52">
         <f t="shared" si="0"/>
         <v>41751</v>
       </c>
-      <c r="AW2" s="104">
+      <c r="AW2" s="52">
         <f t="shared" si="0"/>
         <v>41752</v>
       </c>
-      <c r="AX2" s="104">
+      <c r="AX2" s="52">
         <f t="shared" si="0"/>
         <v>41753</v>
       </c>
-      <c r="AY2" s="104">
+      <c r="AY2" s="52">
         <f t="shared" si="0"/>
         <v>41754</v>
       </c>
-      <c r="AZ2" s="104">
+      <c r="AZ2" s="52">
         <f t="shared" si="0"/>
         <v>41755</v>
       </c>
-      <c r="BA2" s="104">
+      <c r="BA2" s="52">
         <f t="shared" si="0"/>
         <v>41756</v>
       </c>
-      <c r="BB2" s="104">
+      <c r="BB2" s="52">
         <f t="shared" si="0"/>
         <v>41757</v>
       </c>
-      <c r="BC2" s="104">
+      <c r="BC2" s="52">
         <f t="shared" si="0"/>
         <v>41758</v>
       </c>
-      <c r="BD2" s="104">
+      <c r="BD2" s="52">
         <f t="shared" si="0"/>
         <v>41759</v>
       </c>
-      <c r="BE2" s="104">
+      <c r="BE2" s="52">
         <f t="shared" si="0"/>
         <v>41760</v>
       </c>
-      <c r="BF2" s="104">
+      <c r="BF2" s="52">
         <f t="shared" si="0"/>
         <v>41761</v>
       </c>
-      <c r="BG2" s="104">
+      <c r="BG2" s="52">
         <f t="shared" si="0"/>
         <v>41762</v>
       </c>
-      <c r="BH2" s="104">
+      <c r="BH2" s="52">
         <f t="shared" si="0"/>
         <v>41763</v>
       </c>
-      <c r="BI2" s="104">
+      <c r="BI2" s="52">
         <f t="shared" si="0"/>
         <v>41764</v>
       </c>
-      <c r="BJ2" s="104">
+      <c r="BJ2" s="52">
         <f t="shared" si="0"/>
         <v>41765</v>
       </c>
-      <c r="BK2" s="104">
+      <c r="BK2" s="52">
         <f t="shared" si="0"/>
         <v>41766</v>
       </c>
-      <c r="BL2" s="104">
+      <c r="BL2" s="52">
         <f t="shared" si="0"/>
         <v>41767</v>
       </c>
-      <c r="BM2" s="104">
+      <c r="BM2" s="52">
         <f t="shared" si="0"/>
         <v>41768</v>
       </c>
-      <c r="BN2" s="104">
+      <c r="BN2" s="52">
         <f t="shared" si="0"/>
         <v>41769</v>
       </c>
-      <c r="BO2" s="104">
+      <c r="BO2" s="52">
         <f t="shared" si="0"/>
         <v>41770</v>
       </c>
-      <c r="BP2" s="105"/>
-      <c r="BQ2" s="105"/>
-      <c r="BR2" s="105"/>
-      <c r="BS2" s="106"/>
-      <c r="BT2" s="106"/>
-      <c r="BU2" s="106"/>
-      <c r="BV2" s="106"/>
-      <c r="BW2" s="106"/>
-      <c r="BX2" s="106"/>
-      <c r="BY2" s="106"/>
-      <c r="BZ2" s="106"/>
-      <c r="CA2" s="106"/>
-      <c r="CB2" s="106"/>
-      <c r="CC2" s="106"/>
-      <c r="CD2" s="106"/>
+      <c r="BP2" s="53"/>
+      <c r="BQ2" s="53"/>
+      <c r="BR2" s="53"/>
+      <c r="BS2" s="54"/>
+      <c r="BT2" s="54"/>
+      <c r="BU2" s="54"/>
+      <c r="BV2" s="54"/>
+      <c r="BW2" s="54"/>
+      <c r="BX2" s="54"/>
+      <c r="BY2" s="54"/>
+      <c r="BZ2" s="54"/>
+      <c r="CA2" s="54"/>
+      <c r="CB2" s="54"/>
+      <c r="CC2" s="54"/>
+      <c r="CD2" s="54"/>
     </row>
     <row r="3" spans="1:82" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A3" s="7">
@@ -9971,7 +9978,7 @@
       <c r="C7" s="45">
         <v>4</v>
       </c>
-      <c r="D7" s="48"/>
+      <c r="D7" s="108"/>
       <c r="E7" s="21"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
@@ -10213,9 +10220,9 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
+      <c r="N10" s="108"/>
+      <c r="O10" s="108"/>
+      <c r="P10" s="108"/>
       <c r="Q10" s="19"/>
       <c r="R10" s="19"/>
       <c r="S10" s="19"/>
@@ -12203,306 +12210,306 @@
   <sheetData>
     <row r="1" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="53"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="56"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="61"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="56"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="61"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="56"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="61"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="56"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="61"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="56"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="61"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="59"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="64"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="53"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="58"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="56"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="61"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
-      <c r="M13" s="56"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="61"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="56"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="61"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="56"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="61"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="56"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="61"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="56"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="61"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="56"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="61"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B19" s="54"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="55"/>
-      <c r="M19" s="56"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="61"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B20" s="54"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="56"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="61"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B21" s="54"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="56"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="61"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="57"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="59"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="63"/>
+      <c r="M22" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
update schedule based on 15/3/2015 status
</commit_message>
<xml_diff>
--- a/01_doc/proj_plan/餐厅订餐系统_项目计划.xlsx
+++ b/01_doc/proj_plan/餐厅订餐系统_项目计划.xlsx
@@ -547,31 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Lin</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N6" authorId="0" shapeId="0">
+    <comment ref="K6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -620,7 +596,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -644,7 +620,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -668,7 +644,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P10" authorId="0" shapeId="0">
+    <comment ref="G10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -692,7 +668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q11" authorId="0" shapeId="0">
+    <comment ref="H11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -716,7 +692,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T12" authorId="0" shapeId="0">
+    <comment ref="K12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -740,7 +716,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T13" authorId="0" shapeId="0">
+    <comment ref="K13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -764,7 +740,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W14" authorId="0" shapeId="0">
+    <comment ref="N14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -788,7 +764,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z15" authorId="0" shapeId="0">
+    <comment ref="Q15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -812,7 +788,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD16" authorId="0" shapeId="0">
+    <comment ref="J16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -836,7 +812,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD17" authorId="0" shapeId="0">
+    <comment ref="M17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -860,7 +836,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR18" authorId="0" shapeId="0">
+    <comment ref="X18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -884,7 +860,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT19" authorId="0" shapeId="0">
+    <comment ref="Z19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -908,7 +884,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT20" authorId="0" shapeId="0">
+    <comment ref="Z20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -932,7 +908,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BD21" authorId="0" shapeId="0">
+    <comment ref="AJ21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -957,7 +933,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB22" authorId="0" shapeId="0">
+    <comment ref="AH22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -981,7 +957,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB23" authorId="0" shapeId="0">
+    <comment ref="AH23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1999,7 +1975,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2092,6 +2068,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2248,7 +2225,8 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3798,232 +3776,232 @@
   <sheetData>
     <row r="1" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="58"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="59"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="61"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="62"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="61"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="62"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="59"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="61"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="62"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="61"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="62"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B8" s="59"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="61"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="62"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B9" s="62"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="64"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="65"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="58"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="59"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B12" s="59"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="61"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="62"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B13" s="59"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="61"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="62"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="59"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="61"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="62"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="61"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="62"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B16" s="59"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="61"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="62"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="62"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="63"/>
-      <c r="L17" s="63"/>
-      <c r="M17" s="64"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4281,700 +4259,700 @@
   <sheetData>
     <row r="1" spans="2:13" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="68"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="68"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="70"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="71"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="68"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="70"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="71"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="70"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="71"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="68"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="68"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="70"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="71"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="70"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="71"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="68"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="70"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="71"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="73"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="74"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="75" t="s">
         <v>171</v>
       </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="77"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="77"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="79"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="80"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="77"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="78"/>
-      <c r="M16" s="79"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="80"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
-      <c r="K17" s="78"/>
-      <c r="L17" s="78"/>
-      <c r="M17" s="79"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="80"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="77"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="78"/>
-      <c r="L18" s="78"/>
-      <c r="M18" s="79"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="80"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="77"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="78"/>
-      <c r="M19" s="79"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="80"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="77"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="78"/>
-      <c r="M20" s="79"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="80"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="77"/>
-      <c r="C21" s="78"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="78"/>
-      <c r="M21" s="79"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="80"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="77"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="78"/>
-      <c r="M22" s="79"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
+      <c r="M22" s="80"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="77"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="78"/>
-      <c r="M23" s="79"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="80"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="77"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="79"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="80"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="77"/>
-      <c r="C25" s="78"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
-      <c r="J25" s="78"/>
-      <c r="K25" s="78"/>
-      <c r="L25" s="78"/>
-      <c r="M25" s="79"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="79"/>
+      <c r="M25" s="80"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="77"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="78"/>
-      <c r="K26" s="78"/>
-      <c r="L26" s="78"/>
-      <c r="M26" s="79"/>
+      <c r="B26" s="78"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="79"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="79"/>
+      <c r="M26" s="80"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="80"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="81"/>
-      <c r="I27" s="81"/>
-      <c r="J27" s="81"/>
-      <c r="K27" s="81"/>
-      <c r="L27" s="81"/>
-      <c r="M27" s="82"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="83"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="65" t="s">
+      <c r="B28" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="65"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="66"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="66"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="58"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="59"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="59"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="61"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="61"/>
+      <c r="L30" s="61"/>
+      <c r="M30" s="62"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="59"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="61"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="61"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="62"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="59"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="60"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="60"/>
-      <c r="L32" s="60"/>
-      <c r="M32" s="61"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="62"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="59"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="61"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="61"/>
+      <c r="L33" s="61"/>
+      <c r="M33" s="62"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="59"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="60"/>
-      <c r="I34" s="60"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="60"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="61"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="61"/>
+      <c r="M34" s="62"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="62"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="63"/>
-      <c r="J35" s="63"/>
-      <c r="K35" s="63"/>
-      <c r="L35" s="63"/>
-      <c r="M35" s="64"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="65"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="65" t="s">
+      <c r="B36" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="65"/>
-      <c r="L36" s="65"/>
-      <c r="M36" s="65"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="66"/>
+      <c r="J36" s="66"/>
+      <c r="K36" s="66"/>
+      <c r="L36" s="66"/>
+      <c r="M36" s="66"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="74" t="s">
+      <c r="B37" s="75" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="83"/>
-      <c r="M37" s="84"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="84"/>
+      <c r="J37" s="84"/>
+      <c r="K37" s="84"/>
+      <c r="L37" s="84"/>
+      <c r="M37" s="85"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="85"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="86"/>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="86"/>
-      <c r="L38" s="86"/>
-      <c r="M38" s="87"/>
+      <c r="B38" s="86"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="87"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="87"/>
+      <c r="I38" s="87"/>
+      <c r="J38" s="87"/>
+      <c r="K38" s="87"/>
+      <c r="L38" s="87"/>
+      <c r="M38" s="88"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="85"/>
-      <c r="C39" s="86"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="86"/>
-      <c r="F39" s="86"/>
-      <c r="G39" s="86"/>
-      <c r="H39" s="86"/>
-      <c r="I39" s="86"/>
-      <c r="J39" s="86"/>
-      <c r="K39" s="86"/>
-      <c r="L39" s="86"/>
-      <c r="M39" s="87"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="87"/>
+      <c r="E39" s="87"/>
+      <c r="F39" s="87"/>
+      <c r="G39" s="87"/>
+      <c r="H39" s="87"/>
+      <c r="I39" s="87"/>
+      <c r="J39" s="87"/>
+      <c r="K39" s="87"/>
+      <c r="L39" s="87"/>
+      <c r="M39" s="88"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="85"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
-      <c r="E40" s="86"/>
-      <c r="F40" s="86"/>
-      <c r="G40" s="86"/>
-      <c r="H40" s="86"/>
-      <c r="I40" s="86"/>
-      <c r="J40" s="86"/>
-      <c r="K40" s="86"/>
-      <c r="L40" s="86"/>
-      <c r="M40" s="87"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="87"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="87"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="87"/>
+      <c r="I40" s="87"/>
+      <c r="J40" s="87"/>
+      <c r="K40" s="87"/>
+      <c r="L40" s="87"/>
+      <c r="M40" s="88"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="88"/>
-      <c r="C41" s="89"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="89"/>
-      <c r="G41" s="89"/>
-      <c r="H41" s="89"/>
-      <c r="I41" s="89"/>
-      <c r="J41" s="89"/>
-      <c r="K41" s="89"/>
-      <c r="L41" s="89"/>
-      <c r="M41" s="90"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="90"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="90"/>
+      <c r="G41" s="90"/>
+      <c r="H41" s="90"/>
+      <c r="I41" s="90"/>
+      <c r="J41" s="90"/>
+      <c r="K41" s="90"/>
+      <c r="L41" s="90"/>
+      <c r="M41" s="91"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="65" t="s">
+      <c r="B42" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="65"/>
-      <c r="K42" s="65"/>
-      <c r="L42" s="65"/>
-      <c r="M42" s="65"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="66"/>
+      <c r="J42" s="66"/>
+      <c r="K42" s="66"/>
+      <c r="L42" s="66"/>
+      <c r="M42" s="66"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="57"/>
-      <c r="G43" s="57"/>
-      <c r="H43" s="57"/>
-      <c r="I43" s="57"/>
-      <c r="J43" s="57"/>
-      <c r="K43" s="57"/>
-      <c r="L43" s="57"/>
-      <c r="M43" s="58"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="59"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="59"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="60"/>
-      <c r="G44" s="60"/>
-      <c r="H44" s="60"/>
-      <c r="I44" s="60"/>
-      <c r="J44" s="60"/>
-      <c r="K44" s="60"/>
-      <c r="L44" s="60"/>
-      <c r="M44" s="61"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
+      <c r="H44" s="61"/>
+      <c r="I44" s="61"/>
+      <c r="J44" s="61"/>
+      <c r="K44" s="61"/>
+      <c r="L44" s="61"/>
+      <c r="M44" s="62"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="59"/>
-      <c r="C45" s="60"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="60"/>
-      <c r="K45" s="60"/>
-      <c r="L45" s="60"/>
-      <c r="M45" s="61"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
+      <c r="L45" s="61"/>
+      <c r="M45" s="62"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="59"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="60"/>
-      <c r="H46" s="60"/>
-      <c r="I46" s="60"/>
-      <c r="J46" s="60"/>
-      <c r="K46" s="60"/>
-      <c r="L46" s="60"/>
-      <c r="M46" s="61"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="61"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="61"/>
+      <c r="L46" s="61"/>
+      <c r="M46" s="62"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="59"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
-      <c r="K47" s="60"/>
-      <c r="L47" s="60"/>
-      <c r="M47" s="61"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="61"/>
+      <c r="L47" s="61"/>
+      <c r="M47" s="62"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="59"/>
-      <c r="C48" s="60"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="60"/>
-      <c r="F48" s="60"/>
-      <c r="G48" s="60"/>
-      <c r="H48" s="60"/>
-      <c r="I48" s="60"/>
-      <c r="J48" s="60"/>
-      <c r="K48" s="60"/>
-      <c r="L48" s="60"/>
-      <c r="M48" s="61"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="61"/>
+      <c r="L48" s="61"/>
+      <c r="M48" s="62"/>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="62"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="63"/>
-      <c r="H49" s="63"/>
-      <c r="I49" s="63"/>
-      <c r="J49" s="63"/>
-      <c r="K49" s="63"/>
-      <c r="L49" s="63"/>
-      <c r="M49" s="64"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="64"/>
+      <c r="K49" s="64"/>
+      <c r="L49" s="64"/>
+      <c r="M49" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -5023,10 +5001,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
       <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
@@ -5041,10 +5019,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="91">
+      <c r="A3" s="92">
         <v>1</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="92" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="7">
@@ -5067,8 +5045,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="91"/>
-      <c r="B4" s="91"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="7">
         <v>1.2</v>
       </c>
@@ -5089,8 +5067,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="91"/>
-      <c r="B5" s="91"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="92"/>
       <c r="C5" s="7">
         <v>1.3</v>
       </c>
@@ -5111,8 +5089,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="91"/>
-      <c r="B6" s="91"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="7">
         <v>1.4</v>
       </c>
@@ -5133,10 +5111,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="93">
+      <c r="A7" s="94">
         <v>2</v>
       </c>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="92" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="7">
@@ -5159,8 +5137,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="94"/>
-      <c r="B8" s="91"/>
+      <c r="A8" s="95"/>
+      <c r="B8" s="92"/>
       <c r="C8" s="7">
         <v>2.2000000000000002</v>
       </c>
@@ -5181,8 +5159,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="95"/>
-      <c r="B9" s="91"/>
+      <c r="A9" s="96"/>
+      <c r="B9" s="92"/>
       <c r="C9" s="7">
         <v>2.2999999999999998</v>
       </c>
@@ -5203,10 +5181,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="91">
+      <c r="A10" s="92">
         <v>3</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="92" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="9">
@@ -5229,8 +5207,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="91"/>
-      <c r="B11" s="91"/>
+      <c r="A11" s="92"/>
+      <c r="B11" s="92"/>
       <c r="C11" s="9">
         <v>3.2</v>
       </c>
@@ -5251,8 +5229,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="91"/>
-      <c r="B12" s="91"/>
+      <c r="A12" s="92"/>
+      <c r="B12" s="92"/>
       <c r="C12" s="9">
         <v>3.3</v>
       </c>
@@ -5273,8 +5251,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="91"/>
-      <c r="B13" s="91"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="92"/>
       <c r="C13" s="9">
         <v>3.4</v>
       </c>
@@ -5295,8 +5273,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="91"/>
-      <c r="B14" s="91"/>
+      <c r="A14" s="92"/>
+      <c r="B14" s="92"/>
       <c r="C14" s="9">
         <v>3.5</v>
       </c>
@@ -5317,8 +5295,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="91"/>
-      <c r="B15" s="91"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="92"/>
       <c r="C15" s="9">
         <v>3.6</v>
       </c>
@@ -5339,8 +5317,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="91"/>
-      <c r="B16" s="91"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="92"/>
       <c r="C16" s="9">
         <v>3.7</v>
       </c>
@@ -5361,8 +5339,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="91"/>
-      <c r="B17" s="91"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="9">
         <v>3.8</v>
       </c>
@@ -5383,8 +5361,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="91"/>
-      <c r="B18" s="91"/>
+      <c r="A18" s="92"/>
+      <c r="B18" s="92"/>
       <c r="C18" s="9">
         <v>3.9</v>
       </c>
@@ -5405,8 +5383,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="91"/>
-      <c r="B19" s="91"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="92"/>
       <c r="C19" s="9" t="s">
         <v>48</v>
       </c>
@@ -5427,10 +5405,10 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="91">
+      <c r="A20" s="92">
         <v>4</v>
       </c>
-      <c r="B20" s="93" t="s">
+      <c r="B20" s="94" t="s">
         <v>50</v>
       </c>
       <c r="C20" s="7">
@@ -5453,8 +5431,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="91"/>
-      <c r="B21" s="94"/>
+      <c r="A21" s="92"/>
+      <c r="B21" s="95"/>
       <c r="C21" s="7">
         <v>4.2</v>
       </c>
@@ -5475,8 +5453,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="91"/>
-      <c r="B22" s="94"/>
+      <c r="A22" s="92"/>
+      <c r="B22" s="95"/>
       <c r="C22" s="7">
         <v>4.3</v>
       </c>
@@ -5497,8 +5475,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23" s="91"/>
-      <c r="B23" s="94"/>
+      <c r="A23" s="92"/>
+      <c r="B23" s="95"/>
       <c r="C23" s="7">
         <v>4.4000000000000004</v>
       </c>
@@ -5519,8 +5497,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="91"/>
-      <c r="B24" s="94"/>
+      <c r="A24" s="92"/>
+      <c r="B24" s="95"/>
       <c r="C24" s="7">
         <v>4.5</v>
       </c>
@@ -5541,8 +5519,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="91"/>
-      <c r="B25" s="94"/>
+      <c r="A25" s="92"/>
+      <c r="B25" s="95"/>
       <c r="C25" s="7">
         <v>4.5999999999999996</v>
       </c>
@@ -5563,10 +5541,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="91">
+      <c r="A26" s="92">
         <v>5</v>
       </c>
-      <c r="B26" s="91" t="s">
+      <c r="B26" s="92" t="s">
         <v>57</v>
       </c>
       <c r="C26" s="7">
@@ -5589,8 +5567,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A27" s="91"/>
-      <c r="B27" s="91"/>
+      <c r="A27" s="92"/>
+      <c r="B27" s="92"/>
       <c r="C27" s="7">
         <v>5.2</v>
       </c>
@@ -5611,8 +5589,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="91"/>
-      <c r="B28" s="91"/>
+      <c r="A28" s="92"/>
+      <c r="B28" s="92"/>
       <c r="C28" s="7">
         <v>5.3</v>
       </c>
@@ -5633,8 +5611,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="91"/>
-      <c r="B29" s="91"/>
+      <c r="A29" s="92"/>
+      <c r="B29" s="92"/>
       <c r="C29" s="7">
         <v>5.4</v>
       </c>
@@ -5655,8 +5633,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="91"/>
-      <c r="B30" s="91"/>
+      <c r="A30" s="92"/>
+      <c r="B30" s="92"/>
       <c r="C30" s="7">
         <v>5.5</v>
       </c>
@@ -5677,10 +5655,10 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A31" s="91">
+      <c r="A31" s="92">
         <v>6</v>
       </c>
-      <c r="B31" s="91" t="s">
+      <c r="B31" s="92" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="7">
@@ -5703,8 +5681,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="91"/>
-      <c r="B32" s="91"/>
+      <c r="A32" s="92"/>
+      <c r="B32" s="92"/>
       <c r="C32" s="7">
         <v>6.2</v>
       </c>
@@ -5725,8 +5703,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A33" s="91"/>
-      <c r="B33" s="91"/>
+      <c r="A33" s="92"/>
+      <c r="B33" s="92"/>
       <c r="C33" s="7">
         <v>6.3</v>
       </c>
@@ -5747,8 +5725,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="91"/>
-      <c r="B34" s="91"/>
+      <c r="A34" s="92"/>
+      <c r="B34" s="92"/>
       <c r="C34" s="7">
         <v>6.4</v>
       </c>
@@ -5769,8 +5747,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A35" s="91"/>
-      <c r="B35" s="91"/>
+      <c r="A35" s="92"/>
+      <c r="B35" s="92"/>
       <c r="C35" s="7">
         <v>6.5</v>
       </c>
@@ -5791,8 +5769,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A36" s="91"/>
-      <c r="B36" s="91"/>
+      <c r="A36" s="92"/>
+      <c r="B36" s="92"/>
       <c r="C36" s="7">
         <v>6.6</v>
       </c>
@@ -5813,10 +5791,10 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A37" s="91">
+      <c r="A37" s="92">
         <v>7</v>
       </c>
-      <c r="B37" s="91" t="s">
+      <c r="B37" s="92" t="s">
         <v>154</v>
       </c>
       <c r="C37" s="7">
@@ -5839,8 +5817,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A38" s="91"/>
-      <c r="B38" s="91"/>
+      <c r="A38" s="92"/>
+      <c r="B38" s="92"/>
       <c r="C38" s="7">
         <v>7.2</v>
       </c>
@@ -5861,8 +5839,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39" s="91"/>
-      <c r="B39" s="91"/>
+      <c r="A39" s="92"/>
+      <c r="B39" s="92"/>
       <c r="C39" s="7">
         <v>7.3</v>
       </c>
@@ -5883,8 +5861,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="91"/>
-      <c r="B40" s="91"/>
+      <c r="A40" s="92"/>
+      <c r="B40" s="92"/>
       <c r="C40" s="7">
         <v>7.4</v>
       </c>
@@ -5905,8 +5883,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A41" s="91"/>
-      <c r="B41" s="91"/>
+      <c r="A41" s="92"/>
+      <c r="B41" s="92"/>
       <c r="C41" s="7">
         <v>7.5</v>
       </c>
@@ -6544,60 +6522,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="101"/>
-      <c r="B1" s="101"/>
-      <c r="C1" s="103" t="s">
+      <c r="A1" s="102"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="96" t="s">
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
-      <c r="X1" s="97"/>
-      <c r="Y1" s="97"/>
-      <c r="Z1" s="97"/>
-      <c r="AA1" s="97"/>
-      <c r="AB1" s="97"/>
-      <c r="AC1" s="97"/>
-      <c r="AD1" s="97"/>
-      <c r="AE1" s="97"/>
-      <c r="AF1" s="97"/>
-      <c r="AG1" s="97"/>
-      <c r="AH1" s="97"/>
-      <c r="AI1" s="97"/>
-      <c r="AJ1" s="97"/>
-      <c r="AK1" s="97"/>
-      <c r="AL1" s="97"/>
-      <c r="AM1" s="97"/>
-      <c r="AN1" s="97"/>
-      <c r="AO1" s="97"/>
-      <c r="AP1" s="97"/>
-      <c r="AQ1" s="97"/>
-      <c r="AR1" s="97"/>
-      <c r="AS1" s="97"/>
-      <c r="AT1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98"/>
+      <c r="Z1" s="98"/>
+      <c r="AA1" s="98"/>
+      <c r="AB1" s="98"/>
+      <c r="AC1" s="98"/>
+      <c r="AD1" s="98"/>
+      <c r="AE1" s="98"/>
+      <c r="AF1" s="98"/>
+      <c r="AG1" s="98"/>
+      <c r="AH1" s="98"/>
+      <c r="AI1" s="98"/>
+      <c r="AJ1" s="98"/>
+      <c r="AK1" s="98"/>
+      <c r="AL1" s="98"/>
+      <c r="AM1" s="98"/>
+      <c r="AN1" s="98"/>
+      <c r="AO1" s="98"/>
+      <c r="AP1" s="98"/>
+      <c r="AQ1" s="98"/>
+      <c r="AR1" s="98"/>
+      <c r="AS1" s="98"/>
+      <c r="AT1" s="99"/>
     </row>
     <row r="2" spans="1:58" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="102"/>
-      <c r="B2" s="102"/>
+      <c r="A2" s="103"/>
+      <c r="B2" s="103"/>
       <c r="C2" s="16">
         <v>18</v>
       </c>
@@ -6750,9 +6728,9 @@
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -9265,10 +9243,10 @@
   <dimension ref="A1:CD26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N10" sqref="N10:P10"/>
+      <selection pane="bottomRight" activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9284,91 +9262,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:82" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="107" t="s">
+      <c r="B1" s="107"/>
+      <c r="C1" s="108" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="104" t="s">
+      <c r="D1" s="105" t="s">
         <v>172</v>
       </c>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="104"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="104"/>
-      <c r="R1" s="104"/>
-      <c r="S1" s="104"/>
-      <c r="T1" s="104"/>
-      <c r="U1" s="104"/>
-      <c r="V1" s="104"/>
-      <c r="W1" s="104"/>
-      <c r="X1" s="104"/>
-      <c r="Y1" s="104"/>
-      <c r="Z1" s="104"/>
-      <c r="AA1" s="105" t="s">
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="105"/>
+      <c r="W1" s="105"/>
+      <c r="X1" s="105"/>
+      <c r="Y1" s="105"/>
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="106" t="s">
         <v>173</v>
       </c>
-      <c r="AB1" s="105"/>
-      <c r="AC1" s="105"/>
-      <c r="AD1" s="105"/>
-      <c r="AE1" s="105"/>
-      <c r="AF1" s="105"/>
-      <c r="AG1" s="105"/>
-      <c r="AH1" s="105"/>
-      <c r="AI1" s="105"/>
-      <c r="AJ1" s="105"/>
-      <c r="AK1" s="105"/>
-      <c r="AL1" s="105"/>
-      <c r="AM1" s="105"/>
-      <c r="AN1" s="105"/>
-      <c r="AO1" s="105"/>
-      <c r="AP1" s="105"/>
-      <c r="AQ1" s="105"/>
-      <c r="AR1" s="105"/>
-      <c r="AS1" s="105"/>
-      <c r="AT1" s="105"/>
-      <c r="AU1" s="105"/>
-      <c r="AV1" s="105"/>
-      <c r="AW1" s="105"/>
-      <c r="AX1" s="105"/>
-      <c r="AY1" s="105"/>
-      <c r="AZ1" s="105"/>
-      <c r="BA1" s="105"/>
-      <c r="BB1" s="105"/>
-      <c r="BC1" s="105"/>
-      <c r="BD1" s="105"/>
-      <c r="BE1" s="105" t="s">
+      <c r="AB1" s="106"/>
+      <c r="AC1" s="106"/>
+      <c r="AD1" s="106"/>
+      <c r="AE1" s="106"/>
+      <c r="AF1" s="106"/>
+      <c r="AG1" s="106"/>
+      <c r="AH1" s="106"/>
+      <c r="AI1" s="106"/>
+      <c r="AJ1" s="106"/>
+      <c r="AK1" s="106"/>
+      <c r="AL1" s="106"/>
+      <c r="AM1" s="106"/>
+      <c r="AN1" s="106"/>
+      <c r="AO1" s="106"/>
+      <c r="AP1" s="106"/>
+      <c r="AQ1" s="106"/>
+      <c r="AR1" s="106"/>
+      <c r="AS1" s="106"/>
+      <c r="AT1" s="106"/>
+      <c r="AU1" s="106"/>
+      <c r="AV1" s="106"/>
+      <c r="AW1" s="106"/>
+      <c r="AX1" s="106"/>
+      <c r="AY1" s="106"/>
+      <c r="AZ1" s="106"/>
+      <c r="BA1" s="106"/>
+      <c r="BB1" s="106"/>
+      <c r="BC1" s="106"/>
+      <c r="BD1" s="106"/>
+      <c r="BE1" s="106" t="s">
         <v>188</v>
       </c>
-      <c r="BF1" s="105"/>
-      <c r="BG1" s="105"/>
-      <c r="BH1" s="105"/>
-      <c r="BI1" s="105"/>
-      <c r="BJ1" s="105"/>
-      <c r="BK1" s="105"/>
-      <c r="BL1" s="105"/>
-      <c r="BM1" s="105"/>
-      <c r="BN1" s="105"/>
-      <c r="BO1" s="105"/>
-      <c r="BP1" s="105"/>
-      <c r="BQ1" s="105"/>
-      <c r="BR1" s="105"/>
+      <c r="BF1" s="106"/>
+      <c r="BG1" s="106"/>
+      <c r="BH1" s="106"/>
+      <c r="BI1" s="106"/>
+      <c r="BJ1" s="106"/>
+      <c r="BK1" s="106"/>
+      <c r="BL1" s="106"/>
+      <c r="BM1" s="106"/>
+      <c r="BN1" s="106"/>
+      <c r="BO1" s="106"/>
+      <c r="BP1" s="106"/>
+      <c r="BQ1" s="106"/>
+      <c r="BR1" s="106"/>
     </row>
     <row r="2" spans="1:82" s="55" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="106"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="107"/>
+      <c r="A2" s="107"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="108"/>
       <c r="D2" s="51">
         <v>41707</v>
       </c>
@@ -9650,8 +9628,8 @@
       <c r="C3" s="45">
         <v>8</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
       <c r="F3" s="49"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -9709,9 +9687,6 @@
       <c r="BH3" s="19"/>
       <c r="BI3" s="19"/>
       <c r="BJ3" s="19"/>
-      <c r="BK3" s="19"/>
-      <c r="BL3" s="19"/>
-      <c r="BM3" s="19"/>
       <c r="BN3" s="19"/>
       <c r="BO3" s="19"/>
       <c r="BP3" s="19"/>
@@ -9734,14 +9709,14 @@
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="48"/>
+      <c r="F4" s="56"/>
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
       <c r="I4" s="50"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="19"/>
       <c r="O4" s="19"/>
       <c r="P4" s="19"/>
@@ -9784,16 +9759,6 @@
       <c r="BA4" s="19"/>
       <c r="BB4" s="19"/>
       <c r="BC4" s="19"/>
-      <c r="BD4" s="19"/>
-      <c r="BE4" s="19"/>
-      <c r="BF4" s="19"/>
-      <c r="BG4" s="19"/>
-      <c r="BH4" s="19"/>
-      <c r="BI4" s="19"/>
-      <c r="BJ4" s="19"/>
-      <c r="BK4" s="19"/>
-      <c r="BL4" s="19"/>
-      <c r="BM4" s="19"/>
       <c r="BN4" s="19"/>
       <c r="BO4" s="19"/>
       <c r="BP4" s="19"/>
@@ -9817,27 +9782,27 @@
       <c r="D5" s="20"/>
       <c r="E5" s="21"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
       <c r="N5" s="50"/>
       <c r="O5" s="50"/>
       <c r="P5" s="50"/>
       <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="50"/>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
       <c r="AB5" s="19"/>
       <c r="AC5" s="19"/>
       <c r="AD5" s="19"/>
@@ -9866,16 +9831,6 @@
       <c r="BA5" s="19"/>
       <c r="BB5" s="19"/>
       <c r="BC5" s="19"/>
-      <c r="BD5" s="19"/>
-      <c r="BE5" s="19"/>
-      <c r="BF5" s="19"/>
-      <c r="BG5" s="19"/>
-      <c r="BH5" s="19"/>
-      <c r="BI5" s="19"/>
-      <c r="BJ5" s="19"/>
-      <c r="BK5" s="19"/>
-      <c r="BL5" s="19"/>
-      <c r="BM5" s="19"/>
       <c r="BN5" s="19"/>
       <c r="BO5" s="19"/>
       <c r="BP5" s="19"/>
@@ -9899,27 +9854,27 @@
       <c r="D6" s="20"/>
       <c r="E6" s="21"/>
       <c r="F6" s="19"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
       <c r="N6" s="48"/>
       <c r="O6" s="48"/>
       <c r="P6" s="48"/>
       <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="48"/>
-      <c r="T6" s="48"/>
-      <c r="U6" s="48"/>
-      <c r="V6" s="48"/>
-      <c r="W6" s="48"/>
-      <c r="X6" s="48"/>
-      <c r="Y6" s="48"/>
-      <c r="Z6" s="48"/>
-      <c r="AA6" s="48"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
       <c r="AB6" s="19"/>
       <c r="AC6" s="19"/>
       <c r="AD6" s="19"/>
@@ -9938,26 +9893,6 @@
       <c r="AQ6" s="19"/>
       <c r="AR6" s="19"/>
       <c r="AS6" s="19"/>
-      <c r="AT6" s="19"/>
-      <c r="AU6" s="19"/>
-      <c r="AV6" s="19"/>
-      <c r="AW6" s="19"/>
-      <c r="AX6" s="19"/>
-      <c r="AY6" s="19"/>
-      <c r="AZ6" s="19"/>
-      <c r="BA6" s="19"/>
-      <c r="BB6" s="19"/>
-      <c r="BC6" s="19"/>
-      <c r="BD6" s="19"/>
-      <c r="BE6" s="19"/>
-      <c r="BF6" s="19"/>
-      <c r="BG6" s="19"/>
-      <c r="BH6" s="19"/>
-      <c r="BI6" s="19"/>
-      <c r="BJ6" s="19"/>
-      <c r="BK6" s="19"/>
-      <c r="BL6" s="19"/>
-      <c r="BM6" s="19"/>
       <c r="BN6" s="19"/>
       <c r="BO6" s="19"/>
       <c r="BP6" s="19"/>
@@ -9978,29 +9913,30 @@
       <c r="C7" s="45">
         <v>4</v>
       </c>
-      <c r="D7" s="108"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="21"/>
+      <c r="F7" s="109"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
       <c r="AB7" s="19"/>
       <c r="AC7" s="19"/>
       <c r="AD7" s="19"/>
@@ -10019,26 +9955,6 @@
       <c r="AQ7" s="19"/>
       <c r="AR7" s="19"/>
       <c r="AS7" s="19"/>
-      <c r="AT7" s="19"/>
-      <c r="AU7" s="19"/>
-      <c r="AV7" s="19"/>
-      <c r="AW7" s="19"/>
-      <c r="AX7" s="19"/>
-      <c r="AY7" s="19"/>
-      <c r="AZ7" s="19"/>
-      <c r="BA7" s="19"/>
-      <c r="BB7" s="19"/>
-      <c r="BC7" s="19"/>
-      <c r="BD7" s="19"/>
-      <c r="BE7" s="19"/>
-      <c r="BF7" s="19"/>
-      <c r="BG7" s="19"/>
-      <c r="BH7" s="19"/>
-      <c r="BI7" s="19"/>
-      <c r="BJ7" s="19"/>
-      <c r="BK7" s="19"/>
-      <c r="BL7" s="19"/>
-      <c r="BM7" s="19"/>
       <c r="BN7" s="19"/>
       <c r="BO7" s="19"/>
       <c r="BP7" s="19"/>
@@ -10056,16 +9972,16 @@
         <v>4</v>
       </c>
       <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
+      <c r="G8" s="109"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
-      <c r="N8" s="48"/>
+      <c r="N8" s="19"/>
       <c r="O8" s="19"/>
       <c r="P8" s="19"/>
       <c r="Q8" s="19"/>
@@ -10097,26 +10013,6 @@
       <c r="AQ8" s="19"/>
       <c r="AR8" s="19"/>
       <c r="AS8" s="19"/>
-      <c r="AT8" s="19"/>
-      <c r="AU8" s="19"/>
-      <c r="AV8" s="19"/>
-      <c r="AW8" s="19"/>
-      <c r="AX8" s="19"/>
-      <c r="AY8" s="19"/>
-      <c r="AZ8" s="19"/>
-      <c r="BA8" s="19"/>
-      <c r="BB8" s="19"/>
-      <c r="BC8" s="19"/>
-      <c r="BD8" s="19"/>
-      <c r="BE8" s="19"/>
-      <c r="BF8" s="19"/>
-      <c r="BG8" s="19"/>
-      <c r="BH8" s="19"/>
-      <c r="BI8" s="19"/>
-      <c r="BJ8" s="19"/>
-      <c r="BK8" s="19"/>
-      <c r="BL8" s="19"/>
-      <c r="BM8" s="19"/>
       <c r="BN8" s="19"/>
       <c r="BO8" s="19"/>
       <c r="BP8" s="19"/>
@@ -10134,16 +10030,16 @@
         <v>4</v>
       </c>
       <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="H9" s="18"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
+      <c r="K9" s="18"/>
       <c r="L9" s="19"/>
       <c r="M9" s="19"/>
-      <c r="N9" s="48"/>
+      <c r="N9" s="19"/>
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
@@ -10175,26 +10071,6 @@
       <c r="AQ9" s="19"/>
       <c r="AR9" s="19"/>
       <c r="AS9" s="19"/>
-      <c r="AT9" s="19"/>
-      <c r="AU9" s="19"/>
-      <c r="AV9" s="19"/>
-      <c r="AW9" s="19"/>
-      <c r="AX9" s="19"/>
-      <c r="AY9" s="19"/>
-      <c r="AZ9" s="19"/>
-      <c r="BA9" s="19"/>
-      <c r="BB9" s="19"/>
-      <c r="BC9" s="19"/>
-      <c r="BD9" s="19"/>
-      <c r="BE9" s="19"/>
-      <c r="BF9" s="19"/>
-      <c r="BG9" s="19"/>
-      <c r="BH9" s="19"/>
-      <c r="BI9" s="19"/>
-      <c r="BJ9" s="19"/>
-      <c r="BK9" s="19"/>
-      <c r="BL9" s="19"/>
-      <c r="BM9" s="19"/>
       <c r="BN9" s="19"/>
       <c r="BO9" s="19"/>
       <c r="BP9" s="19"/>
@@ -10213,17 +10089,18 @@
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="21"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
-      <c r="N10" s="108"/>
-      <c r="O10" s="108"/>
-      <c r="P10" s="108"/>
-      <c r="Q10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
       <c r="R10" s="19"/>
       <c r="S10" s="19"/>
       <c r="T10" s="19"/>
@@ -10252,26 +10129,6 @@
       <c r="AQ10" s="19"/>
       <c r="AR10" s="19"/>
       <c r="AS10" s="19"/>
-      <c r="AT10" s="19"/>
-      <c r="AU10" s="19"/>
-      <c r="AV10" s="19"/>
-      <c r="AW10" s="19"/>
-      <c r="AX10" s="19"/>
-      <c r="AY10" s="19"/>
-      <c r="AZ10" s="19"/>
-      <c r="BA10" s="19"/>
-      <c r="BB10" s="19"/>
-      <c r="BC10" s="19"/>
-      <c r="BD10" s="19"/>
-      <c r="BE10" s="19"/>
-      <c r="BF10" s="19"/>
-      <c r="BG10" s="19"/>
-      <c r="BH10" s="19"/>
-      <c r="BI10" s="19"/>
-      <c r="BJ10" s="19"/>
-      <c r="BK10" s="19"/>
-      <c r="BL10" s="19"/>
-      <c r="BM10" s="19"/>
       <c r="BN10" s="19"/>
       <c r="BO10" s="19"/>
       <c r="BP10" s="19"/>
@@ -10292,18 +10149,18 @@
       <c r="E11" s="21"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="110"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="109"/>
+      <c r="M11" s="109"/>
+      <c r="N11" s="109"/>
+      <c r="O11" s="109"/>
+      <c r="P11" s="109"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
       <c r="V11" s="19"/>
@@ -10330,26 +10187,6 @@
       <c r="AQ11" s="19"/>
       <c r="AR11" s="19"/>
       <c r="AS11" s="19"/>
-      <c r="AT11" s="19"/>
-      <c r="AU11" s="19"/>
-      <c r="AV11" s="19"/>
-      <c r="AW11" s="19"/>
-      <c r="AX11" s="19"/>
-      <c r="AY11" s="19"/>
-      <c r="AZ11" s="19"/>
-      <c r="BA11" s="19"/>
-      <c r="BB11" s="19"/>
-      <c r="BC11" s="19"/>
-      <c r="BD11" s="19"/>
-      <c r="BE11" s="19"/>
-      <c r="BF11" s="19"/>
-      <c r="BG11" s="19"/>
-      <c r="BH11" s="19"/>
-      <c r="BI11" s="19"/>
-      <c r="BJ11" s="19"/>
-      <c r="BK11" s="19"/>
-      <c r="BL11" s="19"/>
-      <c r="BM11" s="19"/>
       <c r="BN11" s="19"/>
       <c r="BO11" s="19"/>
       <c r="BP11" s="19"/>
@@ -10373,7 +10210,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
+      <c r="K12" s="48"/>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
@@ -10382,7 +10219,7 @@
       <c r="Q12" s="19"/>
       <c r="R12" s="19"/>
       <c r="S12" s="19"/>
-      <c r="T12" s="48"/>
+      <c r="T12" s="19"/>
       <c r="U12" s="19"/>
       <c r="V12" s="19"/>
       <c r="W12" s="19"/>
@@ -10408,26 +10245,6 @@
       <c r="AQ12" s="19"/>
       <c r="AR12" s="19"/>
       <c r="AS12" s="19"/>
-      <c r="AT12" s="19"/>
-      <c r="AU12" s="19"/>
-      <c r="AV12" s="19"/>
-      <c r="AW12" s="19"/>
-      <c r="AX12" s="19"/>
-      <c r="AY12" s="19"/>
-      <c r="AZ12" s="19"/>
-      <c r="BA12" s="19"/>
-      <c r="BB12" s="19"/>
-      <c r="BC12" s="19"/>
-      <c r="BD12" s="19"/>
-      <c r="BE12" s="19"/>
-      <c r="BF12" s="19"/>
-      <c r="BG12" s="19"/>
-      <c r="BH12" s="19"/>
-      <c r="BI12" s="19"/>
-      <c r="BJ12" s="19"/>
-      <c r="BK12" s="19"/>
-      <c r="BL12" s="19"/>
-      <c r="BM12" s="19"/>
       <c r="BN12" s="19"/>
       <c r="BO12" s="19"/>
       <c r="BP12" s="19"/>
@@ -10451,16 +10268,16 @@
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
+      <c r="K13" s="48"/>
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="109"/>
+      <c r="R13" s="18"/>
       <c r="S13" s="19"/>
-      <c r="T13" s="48"/>
+      <c r="T13" s="19"/>
       <c r="U13" s="19"/>
       <c r="V13" s="19"/>
       <c r="W13" s="19"/>
@@ -10486,26 +10303,6 @@
       <c r="AQ13" s="19"/>
       <c r="AR13" s="19"/>
       <c r="AS13" s="19"/>
-      <c r="AT13" s="19"/>
-      <c r="AU13" s="19"/>
-      <c r="AV13" s="19"/>
-      <c r="AW13" s="19"/>
-      <c r="AX13" s="19"/>
-      <c r="AY13" s="19"/>
-      <c r="AZ13" s="19"/>
-      <c r="BA13" s="19"/>
-      <c r="BB13" s="19"/>
-      <c r="BC13" s="19"/>
-      <c r="BD13" s="19"/>
-      <c r="BE13" s="19"/>
-      <c r="BF13" s="19"/>
-      <c r="BG13" s="19"/>
-      <c r="BH13" s="19"/>
-      <c r="BI13" s="19"/>
-      <c r="BJ13" s="19"/>
-      <c r="BK13" s="19"/>
-      <c r="BL13" s="19"/>
-      <c r="BM13" s="19"/>
       <c r="BN13" s="19"/>
       <c r="BO13" s="19"/>
       <c r="BP13" s="19"/>
@@ -10530,18 +10327,18 @@
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
       <c r="O14" s="19"/>
       <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
       <c r="R14" s="19"/>
       <c r="S14" s="19"/>
       <c r="T14" s="19"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="48"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
       <c r="X14" s="19"/>
       <c r="Y14" s="19"/>
       <c r="Z14" s="19"/>
@@ -10564,26 +10361,6 @@
       <c r="AQ14" s="19"/>
       <c r="AR14" s="19"/>
       <c r="AS14" s="19"/>
-      <c r="AT14" s="19"/>
-      <c r="AU14" s="19"/>
-      <c r="AV14" s="19"/>
-      <c r="AW14" s="19"/>
-      <c r="AX14" s="19"/>
-      <c r="AY14" s="19"/>
-      <c r="AZ14" s="19"/>
-      <c r="BA14" s="19"/>
-      <c r="BB14" s="19"/>
-      <c r="BC14" s="19"/>
-      <c r="BD14" s="19"/>
-      <c r="BE14" s="19"/>
-      <c r="BF14" s="19"/>
-      <c r="BG14" s="19"/>
-      <c r="BH14" s="19"/>
-      <c r="BI14" s="19"/>
-      <c r="BJ14" s="19"/>
-      <c r="BK14" s="19"/>
-      <c r="BL14" s="19"/>
-      <c r="BM14" s="19"/>
       <c r="BN14" s="19"/>
       <c r="BO14" s="19"/>
       <c r="BP14" s="19"/>
@@ -10611,18 +10388,18 @@
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
+      <c r="O15" s="48"/>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="48"/>
       <c r="R15" s="19"/>
       <c r="S15" s="19"/>
       <c r="T15" s="19"/>
       <c r="U15" s="19"/>
       <c r="V15" s="19"/>
       <c r="W15" s="19"/>
-      <c r="X15" s="48"/>
-      <c r="Y15" s="48"/>
-      <c r="Z15" s="48"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
       <c r="AA15" s="19"/>
       <c r="AB15" s="19"/>
       <c r="AC15" s="19"/>
@@ -10642,26 +10419,6 @@
       <c r="AQ15" s="19"/>
       <c r="AR15" s="19"/>
       <c r="AS15" s="19"/>
-      <c r="AT15" s="19"/>
-      <c r="AU15" s="19"/>
-      <c r="AV15" s="19"/>
-      <c r="AW15" s="19"/>
-      <c r="AX15" s="19"/>
-      <c r="AY15" s="19"/>
-      <c r="AZ15" s="19"/>
-      <c r="BA15" s="19"/>
-      <c r="BB15" s="19"/>
-      <c r="BC15" s="19"/>
-      <c r="BD15" s="19"/>
-      <c r="BE15" s="19"/>
-      <c r="BF15" s="19"/>
-      <c r="BG15" s="19"/>
-      <c r="BH15" s="19"/>
-      <c r="BI15" s="19"/>
-      <c r="BJ15" s="19"/>
-      <c r="BK15" s="19"/>
-      <c r="BL15" s="19"/>
-      <c r="BM15" s="19"/>
       <c r="BN15" s="19"/>
       <c r="BO15" s="19"/>
       <c r="BP15" s="19"/>
@@ -10682,9 +10439,9 @@
       <c r="E16" s="21"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
@@ -10702,9 +10459,9 @@
       <c r="Y16" s="19"/>
       <c r="Z16" s="19"/>
       <c r="AA16" s="19"/>
-      <c r="AB16" s="48"/>
-      <c r="AC16" s="48"/>
-      <c r="AD16" s="48"/>
+      <c r="AB16" s="19"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="19"/>
       <c r="AE16" s="19"/>
       <c r="AF16" s="19"/>
       <c r="AG16" s="19"/>
@@ -10720,26 +10477,6 @@
       <c r="AQ16" s="19"/>
       <c r="AR16" s="19"/>
       <c r="AS16" s="19"/>
-      <c r="AT16" s="19"/>
-      <c r="AU16" s="19"/>
-      <c r="AV16" s="19"/>
-      <c r="AW16" s="19"/>
-      <c r="AX16" s="19"/>
-      <c r="AY16" s="19"/>
-      <c r="AZ16" s="19"/>
-      <c r="BA16" s="19"/>
-      <c r="BB16" s="19"/>
-      <c r="BC16" s="19"/>
-      <c r="BD16" s="19"/>
-      <c r="BE16" s="19"/>
-      <c r="BF16" s="19"/>
-      <c r="BG16" s="19"/>
-      <c r="BH16" s="19"/>
-      <c r="BI16" s="19"/>
-      <c r="BJ16" s="19"/>
-      <c r="BK16" s="19"/>
-      <c r="BL16" s="19"/>
-      <c r="BM16" s="19"/>
       <c r="BN16" s="19"/>
       <c r="BO16" s="19"/>
       <c r="BP16" s="19"/>
@@ -10763,26 +10500,26 @@
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
       <c r="N17" s="19"/>
       <c r="O17" s="19"/>
       <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="109"/>
+      <c r="S17" s="109"/>
+      <c r="T17" s="109"/>
+      <c r="U17" s="18"/>
       <c r="V17" s="19"/>
       <c r="W17" s="19"/>
       <c r="X17" s="19"/>
       <c r="Y17" s="19"/>
       <c r="Z17" s="19"/>
       <c r="AA17" s="19"/>
-      <c r="AB17" s="48"/>
-      <c r="AC17" s="48"/>
-      <c r="AD17" s="48"/>
+      <c r="AB17" s="19"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="19"/>
       <c r="AE17" s="19"/>
       <c r="AF17" s="19"/>
       <c r="AG17" s="19"/>
@@ -10798,26 +10535,6 @@
       <c r="AQ17" s="19"/>
       <c r="AR17" s="19"/>
       <c r="AS17" s="19"/>
-      <c r="AT17" s="19"/>
-      <c r="AU17" s="19"/>
-      <c r="AV17" s="19"/>
-      <c r="AW17" s="19"/>
-      <c r="AX17" s="19"/>
-      <c r="AY17" s="19"/>
-      <c r="AZ17" s="19"/>
-      <c r="BA17" s="19"/>
-      <c r="BB17" s="19"/>
-      <c r="BC17" s="19"/>
-      <c r="BD17" s="19"/>
-      <c r="BE17" s="19"/>
-      <c r="BF17" s="19"/>
-      <c r="BG17" s="19"/>
-      <c r="BH17" s="19"/>
-      <c r="BI17" s="19"/>
-      <c r="BJ17" s="19"/>
-      <c r="BK17" s="19"/>
-      <c r="BL17" s="19"/>
-      <c r="BM17" s="19"/>
       <c r="BN17" s="19"/>
       <c r="BO17" s="19"/>
       <c r="BP17" s="19"/>
@@ -10841,61 +10558,41 @@
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19"/>
-      <c r="W18" s="19"/>
-      <c r="X18" s="19"/>
-      <c r="Y18" s="19"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="48"/>
+      <c r="W18" s="48"/>
+      <c r="X18" s="48"/>
+      <c r="Y18" s="47"/>
       <c r="Z18" s="19"/>
       <c r="AA18" s="19"/>
       <c r="AB18" s="19"/>
       <c r="AC18" s="19"/>
       <c r="AD18" s="19"/>
-      <c r="AE18" s="48"/>
-      <c r="AF18" s="48"/>
-      <c r="AG18" s="48"/>
-      <c r="AH18" s="48"/>
-      <c r="AI18" s="48"/>
-      <c r="AJ18" s="48"/>
-      <c r="AK18" s="48"/>
-      <c r="AL18" s="48"/>
-      <c r="AM18" s="48"/>
-      <c r="AN18" s="48"/>
-      <c r="AO18" s="48"/>
-      <c r="AP18" s="48"/>
-      <c r="AQ18" s="48"/>
-      <c r="AR18" s="48"/>
-      <c r="AS18" s="47"/>
-      <c r="AT18" s="19"/>
-      <c r="AU18" s="19"/>
-      <c r="AV18" s="19"/>
-      <c r="AW18" s="19"/>
-      <c r="AX18" s="19"/>
-      <c r="AY18" s="19"/>
-      <c r="AZ18" s="19"/>
-      <c r="BA18" s="19"/>
-      <c r="BB18" s="19"/>
-      <c r="BC18" s="19"/>
-      <c r="BD18" s="19"/>
-      <c r="BE18" s="19"/>
-      <c r="BF18" s="19"/>
-      <c r="BG18" s="19"/>
-      <c r="BH18" s="19"/>
-      <c r="BI18" s="19"/>
-      <c r="BJ18" s="19"/>
-      <c r="BK18" s="19"/>
-      <c r="BL18" s="19"/>
-      <c r="BM18" s="19"/>
+      <c r="AE18" s="19"/>
+      <c r="AF18" s="19"/>
+      <c r="AG18" s="19"/>
+      <c r="AH18" s="19"/>
+      <c r="AI18" s="19"/>
+      <c r="AJ18" s="19"/>
+      <c r="AK18" s="19"/>
+      <c r="AL18" s="19"/>
+      <c r="AM18" s="19"/>
+      <c r="AN18" s="19"/>
+      <c r="AO18" s="19"/>
+      <c r="AP18" s="19"/>
+      <c r="AQ18" s="19"/>
+      <c r="AR18" s="19"/>
+      <c r="AS18" s="19"/>
       <c r="BN18" s="19"/>
       <c r="BO18" s="19"/>
       <c r="BP18" s="19"/>
@@ -10933,8 +10630,8 @@
       <c r="V19" s="19"/>
       <c r="W19" s="19"/>
       <c r="X19" s="19"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="19"/>
+      <c r="Y19" s="48"/>
+      <c r="Z19" s="48"/>
       <c r="AA19" s="19"/>
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
@@ -10953,27 +10650,7 @@
       <c r="AP19" s="19"/>
       <c r="AQ19" s="19"/>
       <c r="AR19" s="19"/>
-      <c r="AS19" s="48"/>
-      <c r="AT19" s="48"/>
-      <c r="AU19" s="19"/>
-      <c r="AV19" s="19"/>
-      <c r="AW19" s="19"/>
-      <c r="AX19" s="19"/>
-      <c r="AY19" s="19"/>
-      <c r="AZ19" s="19"/>
-      <c r="BA19" s="19"/>
-      <c r="BB19" s="19"/>
-      <c r="BC19" s="19"/>
-      <c r="BD19" s="19"/>
-      <c r="BE19" s="19"/>
-      <c r="BF19" s="19"/>
-      <c r="BG19" s="19"/>
-      <c r="BH19" s="19"/>
-      <c r="BI19" s="19"/>
-      <c r="BJ19" s="19"/>
-      <c r="BK19" s="19"/>
-      <c r="BL19" s="19"/>
-      <c r="BM19" s="19"/>
+      <c r="AS19" s="19"/>
       <c r="BN19" s="19"/>
       <c r="BO19" s="19"/>
       <c r="BP19" s="19"/>
@@ -11011,8 +10688,8 @@
       <c r="V20" s="19"/>
       <c r="W20" s="19"/>
       <c r="X20" s="19"/>
-      <c r="Y20" s="19"/>
-      <c r="Z20" s="19"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
       <c r="AA20" s="19"/>
       <c r="AB20" s="19"/>
       <c r="AC20" s="19"/>
@@ -11031,27 +10708,7 @@
       <c r="AP20" s="19"/>
       <c r="AQ20" s="19"/>
       <c r="AR20" s="19"/>
-      <c r="AS20" s="48"/>
-      <c r="AT20" s="48"/>
-      <c r="AU20" s="19"/>
-      <c r="AV20" s="19"/>
-      <c r="AW20" s="19"/>
-      <c r="AX20" s="19"/>
-      <c r="AY20" s="19"/>
-      <c r="AZ20" s="19"/>
-      <c r="BA20" s="19"/>
-      <c r="BB20" s="19"/>
-      <c r="BC20" s="19"/>
-      <c r="BD20" s="19"/>
-      <c r="BE20" s="19"/>
-      <c r="BF20" s="19"/>
-      <c r="BG20" s="19"/>
-      <c r="BH20" s="19"/>
-      <c r="BI20" s="19"/>
-      <c r="BJ20" s="19"/>
-      <c r="BK20" s="19"/>
-      <c r="BL20" s="19"/>
-      <c r="BM20" s="19"/>
+      <c r="AS20" s="19"/>
       <c r="BN20" s="19"/>
       <c r="BO20" s="19"/>
       <c r="BP20" s="19"/>
@@ -11078,9 +10735,10 @@
       <c r="K21" s="19"/>
       <c r="L21" s="19"/>
       <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
+      <c r="N21" s="109"/>
       <c r="O21" s="19"/>
       <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
       <c r="R21" s="19"/>
       <c r="S21" s="19"/>
       <c r="T21" s="19"/>
@@ -11090,16 +10748,16 @@
       <c r="X21" s="19"/>
       <c r="Y21" s="19"/>
       <c r="Z21" s="19"/>
-      <c r="AA21" s="19"/>
-      <c r="AB21" s="19"/>
-      <c r="AC21" s="19"/>
-      <c r="AD21" s="19"/>
-      <c r="AE21" s="19"/>
-      <c r="AF21" s="19"/>
-      <c r="AG21" s="19"/>
-      <c r="AH21" s="19"/>
-      <c r="AI21" s="19"/>
-      <c r="AJ21" s="19"/>
+      <c r="AA21" s="48"/>
+      <c r="AB21" s="48"/>
+      <c r="AC21" s="48"/>
+      <c r="AD21" s="48"/>
+      <c r="AE21" s="48"/>
+      <c r="AF21" s="48"/>
+      <c r="AG21" s="48"/>
+      <c r="AH21" s="48"/>
+      <c r="AI21" s="48"/>
+      <c r="AJ21" s="48"/>
       <c r="AK21" s="19"/>
       <c r="AL21" s="19"/>
       <c r="AM21" s="19"/>
@@ -11109,26 +10767,6 @@
       <c r="AQ21" s="19"/>
       <c r="AR21" s="19"/>
       <c r="AS21" s="19"/>
-      <c r="AT21" s="19"/>
-      <c r="AU21" s="48"/>
-      <c r="AV21" s="48"/>
-      <c r="AW21" s="48"/>
-      <c r="AX21" s="48"/>
-      <c r="AY21" s="48"/>
-      <c r="AZ21" s="48"/>
-      <c r="BA21" s="48"/>
-      <c r="BB21" s="48"/>
-      <c r="BC21" s="48"/>
-      <c r="BD21" s="48"/>
-      <c r="BE21" s="19"/>
-      <c r="BF21" s="19"/>
-      <c r="BG21" s="19"/>
-      <c r="BH21" s="19"/>
-      <c r="BI21" s="19"/>
-      <c r="BJ21" s="19"/>
-      <c r="BK21" s="19"/>
-      <c r="BL21" s="19"/>
-      <c r="BM21" s="19"/>
       <c r="BN21" s="19"/>
       <c r="BO21" s="19"/>
       <c r="BP21" s="19"/>
@@ -11174,8 +10812,8 @@
       <c r="AD22" s="19"/>
       <c r="AE22" s="19"/>
       <c r="AF22" s="19"/>
-      <c r="AG22" s="19"/>
-      <c r="AH22" s="19"/>
+      <c r="AG22" s="48"/>
+      <c r="AH22" s="48"/>
       <c r="AI22" s="19"/>
       <c r="AJ22" s="19"/>
       <c r="AK22" s="19"/>
@@ -11187,26 +10825,6 @@
       <c r="AQ22" s="19"/>
       <c r="AR22" s="19"/>
       <c r="AS22" s="19"/>
-      <c r="AT22" s="19"/>
-      <c r="AU22" s="19"/>
-      <c r="AV22" s="19"/>
-      <c r="AW22" s="19"/>
-      <c r="AX22" s="19"/>
-      <c r="AY22" s="19"/>
-      <c r="AZ22" s="19"/>
-      <c r="BA22" s="48"/>
-      <c r="BB22" s="48"/>
-      <c r="BC22" s="19"/>
-      <c r="BD22" s="19"/>
-      <c r="BE22" s="19"/>
-      <c r="BF22" s="19"/>
-      <c r="BG22" s="19"/>
-      <c r="BH22" s="19"/>
-      <c r="BI22" s="19"/>
-      <c r="BJ22" s="19"/>
-      <c r="BK22" s="19"/>
-      <c r="BL22" s="19"/>
-      <c r="BM22" s="19"/>
       <c r="BN22" s="19"/>
       <c r="BO22" s="19"/>
       <c r="BP22" s="19"/>
@@ -11252,8 +10870,8 @@
       <c r="AD23" s="18"/>
       <c r="AE23" s="18"/>
       <c r="AF23" s="18"/>
-      <c r="AG23" s="18"/>
-      <c r="AH23" s="18"/>
+      <c r="AG23" s="48"/>
+      <c r="AH23" s="48"/>
       <c r="AI23" s="18"/>
       <c r="AJ23" s="18"/>
       <c r="AK23" s="18"/>
@@ -11265,26 +10883,6 @@
       <c r="AQ23" s="18"/>
       <c r="AR23" s="18"/>
       <c r="AS23" s="18"/>
-      <c r="AT23" s="18"/>
-      <c r="AU23" s="18"/>
-      <c r="AV23" s="18"/>
-      <c r="AW23" s="18"/>
-      <c r="AX23" s="18"/>
-      <c r="AY23" s="18"/>
-      <c r="AZ23" s="18"/>
-      <c r="BA23" s="48"/>
-      <c r="BB23" s="48"/>
-      <c r="BC23" s="18"/>
-      <c r="BD23" s="18"/>
-      <c r="BE23" s="18"/>
-      <c r="BF23" s="18"/>
-      <c r="BG23" s="18"/>
-      <c r="BH23" s="18"/>
-      <c r="BI23" s="18"/>
-      <c r="BJ23" s="18"/>
-      <c r="BK23" s="18"/>
-      <c r="BL23" s="18"/>
-      <c r="BM23" s="18"/>
       <c r="BN23" s="18"/>
       <c r="BO23" s="18"/>
       <c r="BP23" s="18"/>
@@ -11332,35 +10930,17 @@
       <c r="AF24" s="19"/>
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
-      <c r="AI24" s="19"/>
-      <c r="AJ24" s="19"/>
-      <c r="AK24" s="19"/>
-      <c r="AL24" s="19"/>
-      <c r="AM24" s="19"/>
-      <c r="AN24" s="19"/>
-      <c r="AO24" s="19"/>
+      <c r="AI24" s="48"/>
+      <c r="AJ24" s="48"/>
+      <c r="AK24" s="48"/>
+      <c r="AL24" s="48"/>
+      <c r="AM24" s="48"/>
+      <c r="AN24" s="109"/>
+      <c r="AO24" s="109"/>
       <c r="AP24" s="19"/>
       <c r="AQ24" s="19"/>
       <c r="AR24" s="19"/>
       <c r="AS24" s="19"/>
-      <c r="AT24" s="19"/>
-      <c r="AU24" s="19"/>
-      <c r="AV24" s="19"/>
-      <c r="AW24" s="19"/>
-      <c r="AX24" s="19"/>
-      <c r="AY24" s="19"/>
-      <c r="AZ24" s="19"/>
-      <c r="BA24" s="19"/>
-      <c r="BB24" s="19"/>
-      <c r="BC24" s="48"/>
-      <c r="BD24" s="48"/>
-      <c r="BE24" s="48"/>
-      <c r="BF24" s="48"/>
-      <c r="BG24" s="48"/>
-      <c r="BJ24" s="19"/>
-      <c r="BK24" s="19"/>
-      <c r="BL24" s="19"/>
-      <c r="BM24" s="19"/>
       <c r="BN24" s="19"/>
       <c r="BO24" s="19"/>
       <c r="BP24" s="19"/>
@@ -11413,30 +10993,12 @@
       <c r="AK25" s="19"/>
       <c r="AL25" s="19"/>
       <c r="AM25" s="19"/>
-      <c r="AN25" s="19"/>
-      <c r="AO25" s="19"/>
-      <c r="AP25" s="19"/>
-      <c r="AQ25" s="19"/>
-      <c r="AR25" s="19"/>
-      <c r="AS25" s="19"/>
-      <c r="AT25" s="19"/>
-      <c r="AU25" s="19"/>
-      <c r="AV25" s="19"/>
-      <c r="AW25" s="19"/>
-      <c r="AX25" s="19"/>
-      <c r="AY25" s="19"/>
-      <c r="AZ25" s="19"/>
-      <c r="BA25" s="19"/>
-      <c r="BB25" s="19"/>
-      <c r="BC25" s="19"/>
-      <c r="BD25" s="19"/>
-      <c r="BE25" s="19"/>
-      <c r="BF25" s="19"/>
-      <c r="BG25" s="19"/>
-      <c r="BH25" s="48"/>
-      <c r="BI25" s="48"/>
-      <c r="BJ25" s="48"/>
-      <c r="BK25" s="48"/>
+      <c r="AN25" s="48"/>
+      <c r="AO25" s="48"/>
+      <c r="AP25" s="48"/>
+      <c r="AQ25" s="48"/>
+      <c r="AR25" s="109"/>
+      <c r="AS25" s="109"/>
       <c r="BN25" s="50"/>
       <c r="BO25" s="50"/>
       <c r="BP25" s="50"/>
@@ -11493,28 +11055,8 @@
       <c r="AO26" s="19"/>
       <c r="AP26" s="19"/>
       <c r="AQ26" s="19"/>
-      <c r="AR26" s="19"/>
-      <c r="AS26" s="19"/>
-      <c r="AT26" s="19"/>
-      <c r="AU26" s="19"/>
-      <c r="AV26" s="19"/>
-      <c r="AW26" s="19"/>
-      <c r="AX26" s="19"/>
-      <c r="AY26" s="19"/>
-      <c r="AZ26" s="19"/>
-      <c r="BA26" s="19"/>
-      <c r="BB26" s="19"/>
-      <c r="BC26" s="19"/>
-      <c r="BD26" s="19"/>
-      <c r="BE26" s="19"/>
-      <c r="BF26" s="19"/>
-      <c r="BG26" s="19"/>
-      <c r="BH26" s="19"/>
-      <c r="BI26" s="19"/>
-      <c r="BJ26" s="19"/>
-      <c r="BK26" s="19"/>
-      <c r="BL26" s="48"/>
-      <c r="BM26" s="48"/>
+      <c r="AR26" s="48"/>
+      <c r="AS26" s="48"/>
       <c r="BN26" s="19"/>
       <c r="BO26" s="19"/>
       <c r="BP26" s="19"/>
@@ -12210,306 +11752,306 @@
   <sheetData>
     <row r="1" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="59"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="61"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="62"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="61"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="62"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="59"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="61"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="62"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="61"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="62"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B8" s="59"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="61"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="62"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B9" s="62"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="64"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="65"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="59"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B12" s="59"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="61"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="62"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B13" s="59"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="61"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="62"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="59"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="61"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="62"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="61"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="62"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B16" s="59"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="61"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="62"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="61"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="62"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="59"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="61"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="62"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B19" s="59"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="61"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="61"/>
+      <c r="L19" s="61"/>
+      <c r="M19" s="62"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B20" s="59"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="61"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="62"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B21" s="59"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="61"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="61"/>
+      <c r="M21" s="62"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="62"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="63"/>
-      <c r="L22" s="63"/>
-      <c r="M22" s="64"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>